<commit_message>
Add raspberry pi-controlled relay circuit
</commit_message>
<xml_diff>
--- a/docs/anchor_DFMEA.xlsx
+++ b/docs/anchor_DFMEA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmatt\Documents\anchor\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F567E11-77FA-4AC8-8910-BED5E5D74DF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEAA4534-711E-49CC-86BD-0B644BEB6096}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{6E08087A-9028-4EA2-B63F-382C2D4CF040}"/>
   </bookViews>
@@ -17,7 +17,6 @@
     <sheet name="AP_lookup_table" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2315" uniqueCount="1156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2315" uniqueCount="1159">
   <si>
     <t>Ref ID</t>
   </si>
@@ -3185,9 +3184,6 @@
     <t>Open circuit mains wire</t>
   </si>
   <si>
-    <t>Open circuit thermistor wire</t>
-  </si>
-  <si>
     <t>No power input to heater</t>
   </si>
   <si>
@@ -3495,6 +3491,18 @@
   </si>
   <si>
     <t>Metal Mount</t>
+  </si>
+  <si>
+    <t>Controller interprets temperature higher than actual</t>
+  </si>
+  <si>
+    <t>Open circuit PTC thermistor wire</t>
+  </si>
+  <si>
+    <t>Open circuit NTC thermistor wire</t>
+  </si>
+  <si>
+    <t>Software bug; Hardware failure / mosfet fused closed</t>
   </si>
 </sst>
 </file>
@@ -3623,6 +3631,12 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -3634,12 +3648,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4008,7 +4016,7 @@
   <dimension ref="A1:P72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4016,7 +4024,7 @@
     <col min="1" max="1" width="9.140625" style="2"/>
     <col min="2" max="2" width="18.140625" style="2" customWidth="1"/>
     <col min="3" max="3" width="18.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="26.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="30.28515625" style="1" customWidth="1"/>
     <col min="7" max="7" width="29.140625" style="1" customWidth="1"/>
@@ -4033,94 +4041,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>1098</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
+      <c r="A1" s="10" t="s">
+        <v>1097</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
       <c r="P1" s="5"/>
     </row>
     <row r="2" spans="1:16" ht="93" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="12" t="s">
+      <c r="B2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="8" t="s">
         <v>1031</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="8" t="s">
         <v>1032</v>
       </c>
-      <c r="H2" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="12" t="s">
+      <c r="H2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" s="12" t="s">
+      <c r="J2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="8" t="s">
         <v>1050</v>
       </c>
-      <c r="L2" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="M2" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="N2" s="12" t="s">
+      <c r="L2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="N2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="P2" s="13" t="s">
+      <c r="O2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="P2" s="9" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
-        <v>1116</v>
-      </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="11"/>
+      <c r="A3" s="11" t="s">
+        <v>1115</v>
+      </c>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="13"/>
     </row>
     <row r="4" spans="1:16" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
@@ -4148,7 +4156,7 @@
         <v>10</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="J4" s="4">
         <v>1</v>
@@ -4188,10 +4196,10 @@
         <v>1051</v>
       </c>
       <c r="E5" s="4" t="s">
+        <v>1052</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>1053</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>1054</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>1027</v>
@@ -4206,7 +4214,7 @@
         <v>2</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="L5" s="4">
         <v>2</v>
@@ -4216,7 +4224,7 @@
         <v>8</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="O5" s="4" t="s">
         <v>12</v>
@@ -4237,13 +4245,13 @@
         <v>5</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>1052</v>
+        <v>1157</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>1027</v>
@@ -4258,7 +4266,7 @@
         <v>2</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="L6" s="4">
         <v>2</v>
@@ -4268,10 +4276,10 @@
         <v>12</v>
       </c>
       <c r="N6" s="4" t="s">
+        <v>1056</v>
+      </c>
+      <c r="O6" s="4" t="s">
         <v>1057</v>
-      </c>
-      <c r="O6" s="4" t="s">
-        <v>1058</v>
       </c>
       <c r="P6" s="4" t="str">
         <f>VLOOKUP((H6&amp;J6&amp;L6),AP_lookup_table!D4:E1003,2,FALSE)</f>
@@ -4289,13 +4297,13 @@
         <v>5</v>
       </c>
       <c r="D7" s="4" t="s">
+        <v>1058</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>1059</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="F7" s="4" t="s">
         <v>1060</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>1061</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>1027</v>
@@ -4304,13 +4312,13 @@
         <v>7</v>
       </c>
       <c r="I7" s="4" t="s">
+        <v>1061</v>
+      </c>
+      <c r="J7" s="4">
+        <v>3</v>
+      </c>
+      <c r="K7" s="4" t="s">
         <v>1062</v>
-      </c>
-      <c r="J7" s="4">
-        <v>3</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>1063</v>
       </c>
       <c r="L7" s="4">
         <v>7</v>
@@ -4320,10 +4328,10 @@
         <v>147</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="P7" s="4" t="str">
         <f>VLOOKUP((H7&amp;J7&amp;L7),AP_lookup_table!D5:E1004,2,FALSE)</f>
@@ -4341,13 +4349,13 @@
         <v>5</v>
       </c>
       <c r="D8" s="4" t="s">
+        <v>1066</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>1067</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="F8" s="4" t="s">
         <v>1068</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>1069</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>1027</v>
@@ -4356,13 +4364,13 @@
         <v>6</v>
       </c>
       <c r="I8" s="4" t="s">
+        <v>1069</v>
+      </c>
+      <c r="J8" s="4">
+        <v>2</v>
+      </c>
+      <c r="K8" s="4" t="s">
         <v>1070</v>
-      </c>
-      <c r="J8" s="4">
-        <v>2</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>1071</v>
       </c>
       <c r="L8" s="4">
         <v>3</v>
@@ -4372,10 +4380,10 @@
         <v>36</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="P8" s="4" t="str">
         <f>VLOOKUP((H8&amp;J8&amp;L8),AP_lookup_table!D6:E1005,2,FALSE)</f>
@@ -4396,25 +4404,25 @@
         <v>1047</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="H9" s="4">
         <v>8</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="J9" s="4">
         <v>1</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="L9" s="4">
         <v>5</v>
@@ -4424,10 +4432,10 @@
         <v>40</v>
       </c>
       <c r="N9" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="O9" s="4" t="s">
         <v>1077</v>
-      </c>
-      <c r="O9" s="4" t="s">
-        <v>1078</v>
       </c>
       <c r="P9" s="4" t="str">
         <f>VLOOKUP((H9&amp;J9&amp;L9),AP_lookup_table!D6:E1005,2,FALSE)</f>
@@ -4448,10 +4456,10 @@
         <v>1038</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>1027</v>
@@ -4466,7 +4474,7 @@
         <v>2</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="L10" s="4">
         <v>7</v>
@@ -4479,7 +4487,7 @@
         <v>12</v>
       </c>
       <c r="O10" s="4" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="P10" s="4" t="str">
         <f>VLOOKUP((H10&amp;J10&amp;L10),AP_lookup_table!D7:E1006,2,FALSE)</f>
@@ -4497,28 +4505,28 @@
         <v>1040</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="E11" s="4" t="s">
+        <v>1078</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>1079</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="G11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H11" s="4">
+        <v>10</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>1089</v>
+      </c>
+      <c r="J11" s="4">
+        <v>2</v>
+      </c>
+      <c r="K11" s="4" t="s">
         <v>1080</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H11" s="4">
-        <v>10</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>1090</v>
-      </c>
-      <c r="J11" s="4">
-        <v>2</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>1081</v>
       </c>
       <c r="L11" s="4">
         <v>2</v>
@@ -4528,7 +4536,7 @@
         <v>40</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="O11" s="4" t="s">
         <v>12</v>
@@ -4549,13 +4557,13 @@
         <v>1040</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="E12" s="4" t="s">
+        <v>1090</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>1091</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>1092</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>1027</v>
@@ -4564,13 +4572,13 @@
         <v>1</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="J12" s="4">
         <v>1</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="L12" s="4">
         <v>1</v>
@@ -4580,7 +4588,7 @@
         <v>1</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="O12" s="4" t="s">
         <v>12</v>
@@ -4592,7 +4600,7 @@
     </row>
     <row r="13" spans="1:16" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>1030</v>
@@ -4607,7 +4615,7 @@
         <v>1049</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>3</v>
@@ -4616,13 +4624,13 @@
         <v>10</v>
       </c>
       <c r="I13" s="4" t="s">
+        <v>1082</v>
+      </c>
+      <c r="J13" s="4">
+        <v>3</v>
+      </c>
+      <c r="K13" s="4" t="s">
         <v>1083</v>
-      </c>
-      <c r="J13" s="4">
-        <v>3</v>
-      </c>
-      <c r="K13" s="4" t="s">
-        <v>1084</v>
       </c>
       <c r="L13" s="4">
         <v>2</v>
@@ -4632,7 +4640,7 @@
         <v>60</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="O13" s="4" t="s">
         <v>12</v>
@@ -4653,28 +4661,28 @@
         <v>1041</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="E14" s="4" t="s">
+        <v>1100</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>1098</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>1099</v>
+      </c>
+      <c r="H14" s="4">
+        <v>6</v>
+      </c>
+      <c r="I14" s="4" t="s">
         <v>1101</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>1099</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>1100</v>
-      </c>
-      <c r="H14" s="4">
-        <v>6</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>1102</v>
-      </c>
       <c r="J14" s="4">
         <v>1</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="L14" s="4">
         <v>7</v>
@@ -4684,10 +4692,10 @@
         <v>42</v>
       </c>
       <c r="N14" s="4" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="O14" s="4" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="P14" s="4" t="str">
         <f>VLOOKUP((H14&amp;J14&amp;L14),AP_lookup_table!D11:E1010,2,FALSE)</f>
@@ -4695,34 +4703,34 @@
       </c>
     </row>
     <row r="15" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="9" t="s">
-        <v>1120</v>
-      </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="11"/>
+      <c r="A15" s="11" t="s">
+        <v>1119</v>
+      </c>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="13"/>
     </row>
     <row r="16" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
@@ -4745,34 +4753,34 @@
       </c>
     </row>
     <row r="17" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="9" t="s">
-        <v>1117</v>
-      </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="10"/>
-      <c r="N17" s="10"/>
-      <c r="O17" s="10"/>
-      <c r="P17" s="11"/>
+      <c r="A17" s="11" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
+      <c r="N17" s="12"/>
+      <c r="O17" s="12"/>
+      <c r="P17" s="13"/>
     </row>
     <row r="18" spans="1:16" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="B18" s="4" t="s">
+        <v>1113</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>1114</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>1115</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>1028</v>
@@ -4790,7 +4798,7 @@
         <v>10</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="J18" s="4">
         <v>1</v>
@@ -4818,22 +4826,22 @@
     </row>
     <row r="19" spans="1:16" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>1113</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>1114</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>1115</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>1051</v>
       </c>
       <c r="E19" s="4" t="s">
+        <v>1052</v>
+      </c>
+      <c r="F19" s="4" t="s">
         <v>1053</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>1054</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>1027</v>
@@ -4848,7 +4856,7 @@
         <v>2</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="L19" s="4">
         <v>2</v>
@@ -4858,7 +4866,7 @@
         <v>8</v>
       </c>
       <c r="N19" s="4" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="O19" s="4" t="s">
         <v>12</v>
@@ -4870,22 +4878,22 @@
     </row>
     <row r="20" spans="1:16" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="B20" s="4" t="s">
+        <v>1113</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>1114</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>1115</v>
-      </c>
       <c r="D20" s="4" t="s">
-        <v>1052</v>
+        <v>1156</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>1074</v>
+        <v>1155</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>1027</v>
@@ -4900,7 +4908,7 @@
         <v>2</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="L20" s="4">
         <v>2</v>
@@ -4910,10 +4918,10 @@
         <v>12</v>
       </c>
       <c r="N20" s="4" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="O20" s="4" t="s">
-        <v>1058</v>
+        <v>12</v>
       </c>
       <c r="P20" s="4" t="str">
         <f>VLOOKUP((H20&amp;J20&amp;L20),AP_lookup_table!D15:E1014,2,FALSE)</f>
@@ -4922,22 +4930,22 @@
     </row>
     <row r="21" spans="1:16" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="B21" s="4" t="s">
+        <v>1113</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>1114</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>1115</v>
-      </c>
       <c r="D21" s="4" t="s">
+        <v>1058</v>
+      </c>
+      <c r="E21" s="4" t="s">
         <v>1059</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="F21" s="4" t="s">
         <v>1060</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>1061</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>1027</v>
@@ -4946,13 +4954,13 @@
         <v>7</v>
       </c>
       <c r="I21" s="4" t="s">
+        <v>1061</v>
+      </c>
+      <c r="J21" s="4">
+        <v>3</v>
+      </c>
+      <c r="K21" s="4" t="s">
         <v>1062</v>
-      </c>
-      <c r="J21" s="4">
-        <v>3</v>
-      </c>
-      <c r="K21" s="4" t="s">
-        <v>1063</v>
       </c>
       <c r="L21" s="4">
         <v>7</v>
@@ -4962,10 +4970,10 @@
         <v>147</v>
       </c>
       <c r="N21" s="4" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="O21" s="4" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="P21" s="4" t="str">
         <f>VLOOKUP((H21&amp;J21&amp;L21),AP_lookup_table!D16:E1015,2,FALSE)</f>
@@ -4974,22 +4982,22 @@
     </row>
     <row r="22" spans="1:16" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="B22" s="4" t="s">
+        <v>1113</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>1114</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>1115</v>
-      </c>
       <c r="D22" s="4" t="s">
+        <v>1066</v>
+      </c>
+      <c r="E22" s="4" t="s">
         <v>1067</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="F22" s="4" t="s">
         <v>1068</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>1069</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>1027</v>
@@ -4998,13 +5006,13 @@
         <v>6</v>
       </c>
       <c r="I22" s="4" t="s">
+        <v>1069</v>
+      </c>
+      <c r="J22" s="4">
+        <v>2</v>
+      </c>
+      <c r="K22" s="4" t="s">
         <v>1070</v>
-      </c>
-      <c r="J22" s="4">
-        <v>2</v>
-      </c>
-      <c r="K22" s="4" t="s">
-        <v>1071</v>
       </c>
       <c r="L22" s="4">
         <v>3</v>
@@ -5014,10 +5022,10 @@
         <v>36</v>
       </c>
       <c r="N22" s="4" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="O22" s="4" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="P22" s="4" t="str">
         <f>VLOOKUP((H22&amp;J22&amp;L22),AP_lookup_table!D17:E1016,2,FALSE)</f>
@@ -5026,19 +5034,19 @@
     </row>
     <row r="23" spans="1:16" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="B23" s="4" t="s">
+        <v>1113</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>1114</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>1115</v>
-      </c>
       <c r="D23" s="4" t="s">
+        <v>1144</v>
+      </c>
+      <c r="E23" s="4" t="s">
         <v>1145</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>1146</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>1027</v>
@@ -5050,13 +5058,13 @@
         <v>4</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="J23" s="4">
         <v>2</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="L23" s="4">
         <v>5</v>
@@ -5069,7 +5077,7 @@
         <v>12</v>
       </c>
       <c r="O23" s="4" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="P23" s="4" t="str">
         <f>VLOOKUP((H23&amp;J23&amp;L23),AP_lookup_table!D17:E1016,2,FALSE)</f>
@@ -5078,22 +5086,22 @@
     </row>
     <row r="24" spans="1:16" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>1038</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>1027</v>
@@ -5108,7 +5116,7 @@
         <v>2</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="L24" s="4">
         <v>7</v>
@@ -5121,7 +5129,7 @@
         <v>12</v>
       </c>
       <c r="O24" s="4" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="P24" s="4" t="str">
         <f>VLOOKUP((H24&amp;J24&amp;L24),AP_lookup_table!D18:E1017,2,FALSE)</f>
@@ -5130,37 +5138,37 @@
     </row>
     <row r="25" spans="1:16" ht="66.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>1040</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="E25" s="4" t="s">
+        <v>1078</v>
+      </c>
+      <c r="F25" s="4" t="s">
         <v>1079</v>
       </c>
-      <c r="F25" s="4" t="s">
+      <c r="G25" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H25" s="4">
+        <v>10</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>1089</v>
+      </c>
+      <c r="J25" s="4">
+        <v>2</v>
+      </c>
+      <c r="K25" s="4" t="s">
         <v>1080</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H25" s="4">
-        <v>10</v>
-      </c>
-      <c r="I25" s="4" t="s">
-        <v>1090</v>
-      </c>
-      <c r="J25" s="4">
-        <v>2</v>
-      </c>
-      <c r="K25" s="4" t="s">
-        <v>1081</v>
       </c>
       <c r="L25" s="4">
         <v>2</v>
@@ -5170,7 +5178,7 @@
         <v>40</v>
       </c>
       <c r="N25" s="4" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="O25" s="4" t="s">
         <v>12</v>
@@ -5182,22 +5190,22 @@
     </row>
     <row r="26" spans="1:16" ht="66.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>1040</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="E26" s="4" t="s">
+        <v>1090</v>
+      </c>
+      <c r="F26" s="4" t="s">
         <v>1091</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>1092</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>1027</v>
@@ -5206,13 +5214,13 @@
         <v>1</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="J26" s="4">
         <v>1</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="L26" s="4">
         <v>1</v>
@@ -5222,7 +5230,7 @@
         <v>1</v>
       </c>
       <c r="N26" s="4" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="O26" s="4" t="s">
         <v>12</v>
@@ -5234,10 +5242,10 @@
     </row>
     <row r="27" spans="1:16" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>1040</v>
@@ -5249,7 +5257,7 @@
         <v>1049</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="G27" s="4" t="s">
         <v>3</v>
@@ -5258,13 +5266,13 @@
         <v>10</v>
       </c>
       <c r="I27" s="4" t="s">
+        <v>1082</v>
+      </c>
+      <c r="J27" s="4">
+        <v>3</v>
+      </c>
+      <c r="K27" s="4" t="s">
         <v>1083</v>
-      </c>
-      <c r="J27" s="4">
-        <v>3</v>
-      </c>
-      <c r="K27" s="4" t="s">
-        <v>1084</v>
       </c>
       <c r="L27" s="4">
         <v>2</v>
@@ -5274,7 +5282,7 @@
         <v>60</v>
       </c>
       <c r="N27" s="4" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="O27" s="4" t="s">
         <v>12</v>
@@ -5286,37 +5294,37 @@
     </row>
     <row r="28" spans="1:16" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>1041</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="E28" s="4" t="s">
+        <v>1100</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>1098</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>1099</v>
+      </c>
+      <c r="H28" s="4">
+        <v>6</v>
+      </c>
+      <c r="I28" s="4" t="s">
         <v>1101</v>
       </c>
-      <c r="F28" s="4" t="s">
-        <v>1099</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>1100</v>
-      </c>
-      <c r="H28" s="4">
-        <v>6</v>
-      </c>
-      <c r="I28" s="4" t="s">
-        <v>1102</v>
-      </c>
       <c r="J28" s="4">
         <v>1</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="L28" s="4">
         <v>7</v>
@@ -5326,10 +5334,10 @@
         <v>42</v>
       </c>
       <c r="N28" s="4" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="O28" s="4" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="P28" s="4" t="str">
         <f>VLOOKUP((H28&amp;J28&amp;L28),AP_lookup_table!D22:E1021,2,FALSE)</f>
@@ -5338,37 +5346,37 @@
     </row>
     <row r="29" spans="1:16" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
+        <v>1132</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>1113</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>1133</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>1114</v>
-      </c>
-      <c r="C29" s="4" t="s">
+      <c r="D29" s="4" t="s">
+        <v>1135</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>1138</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>1139</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H29" s="4">
+        <v>5</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>1136</v>
+      </c>
+      <c r="J29" s="4">
+        <v>3</v>
+      </c>
+      <c r="K29" s="4" t="s">
         <v>1134</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>1136</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>1139</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>1140</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>1141</v>
-      </c>
-      <c r="H29" s="4">
-        <v>5</v>
-      </c>
-      <c r="I29" s="4" t="s">
-        <v>1137</v>
-      </c>
-      <c r="J29" s="4">
-        <v>3</v>
-      </c>
-      <c r="K29" s="4" t="s">
-        <v>1135</v>
       </c>
       <c r="L29" s="4">
         <v>2</v>
@@ -5378,7 +5386,7 @@
         <v>30</v>
       </c>
       <c r="N29" s="4" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="O29" s="4" t="s">
         <v>12</v>
@@ -5389,43 +5397,43 @@
       </c>
     </row>
     <row r="30" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="9" t="s">
-        <v>1118</v>
-      </c>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="10"/>
-      <c r="I30" s="10"/>
-      <c r="J30" s="10"/>
-      <c r="K30" s="10"/>
-      <c r="L30" s="10"/>
-      <c r="M30" s="10"/>
-      <c r="N30" s="10"/>
-      <c r="O30" s="10"/>
-      <c r="P30" s="11"/>
+      <c r="A30" s="11" t="s">
+        <v>1117</v>
+      </c>
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="12"/>
+      <c r="M30" s="12"/>
+      <c r="N30" s="12"/>
+      <c r="O30" s="12"/>
+      <c r="P30" s="13"/>
     </row>
     <row r="31" spans="1:16" ht="111" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
+        <v>1103</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>1104</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="C31" s="4" t="s">
+        <v>1111</v>
+      </c>
+      <c r="D31" s="4" t="s">
         <v>1105</v>
       </c>
-      <c r="C31" s="4" t="s">
-        <v>1112</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>1106</v>
-      </c>
       <c r="E31" s="4" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>3</v>
@@ -5434,13 +5442,13 @@
         <v>10</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>1109</v>
+        <v>1158</v>
       </c>
       <c r="J31" s="4">
         <v>2</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="L31" s="4">
         <v>1</v>
@@ -5462,22 +5470,22 @@
     </row>
     <row r="32" spans="1:16" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="G32" s="4" t="s">
         <v>1027</v>
@@ -5486,13 +5494,13 @@
         <v>1</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="J32" s="4">
         <v>1</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="L32" s="4">
         <v>3</v>
@@ -5514,37 +5522,37 @@
     </row>
     <row r="33" spans="1:16" ht="116.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
+        <v>1110</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>1104</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>1111</v>
       </c>
-      <c r="B33" s="4" t="s">
-        <v>1105</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>1112</v>
-      </c>
       <c r="D33" s="4" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="E33" s="4" t="s">
+        <v>1147</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>1151</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H33" s="4">
+        <v>10</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>1150</v>
+      </c>
+      <c r="J33" s="4">
+        <v>2</v>
+      </c>
+      <c r="K33" s="4" t="s">
         <v>1148</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>1152</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H33" s="4">
-        <v>10</v>
-      </c>
-      <c r="I33" s="4" t="s">
-        <v>1151</v>
-      </c>
-      <c r="J33" s="4">
-        <v>2</v>
-      </c>
-      <c r="K33" s="4" t="s">
-        <v>1149</v>
       </c>
       <c r="L33" s="4">
         <v>1</v>
@@ -6276,6 +6284,18 @@
   </mergeCells>
   <conditionalFormatting sqref="H4:H16 J4:J16 L4:L16 L18:L29 J18:J29 H18:H29 L31:L125 H31:H125 J31:J125">
     <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="5"/>
+        <cfvo type="num" val="10"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L16 J16 H16">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="num" val="1"/>
         <cfvo type="num" val="5"/>
@@ -6298,29 +6318,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P4:P16 P18:P29 P31:P125">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
-      <formula>"H"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
-      <formula>"M"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="9" operator="equal">
-      <formula>"L"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J16 L16 H16">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="num" val="1"/>
-        <cfvo type="num" val="5"/>
-        <cfvo type="num" val="10"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="M16">
     <cfRule type="colorScale" priority="1">
       <colorScale>
@@ -6333,14 +6330,25 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P16">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+  <conditionalFormatting sqref="P4:P16">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
       <formula>"M"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula>"L"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P18:P29 P31:P125">
+    <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
+      <formula>"H"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="8" operator="equal">
+      <formula>"M"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="9" operator="equal">
       <formula>"L"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
DFMEA: Finish first draft
</commit_message>
<xml_diff>
--- a/docs/anchor_DFMEA.xlsx
+++ b/docs/anchor_DFMEA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmatt\Documents\anchor\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEAA4534-711E-49CC-86BD-0B644BEB6096}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{227354BB-CF86-4EA9-BBEA-9B40EE7A00CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{6E08087A-9028-4EA2-B63F-382C2D4CF040}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2315" uniqueCount="1159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2496" uniqueCount="1198">
   <si>
     <t>Ref ID</t>
   </si>
@@ -3337,30 +3337,9 @@
     <t>Switch off SSR before switching off contactor &amp; vice versa to minimize spark</t>
   </si>
   <si>
-    <t>4.1.1</t>
-  </si>
-  <si>
-    <t>Controller</t>
-  </si>
-  <si>
-    <t>Controller lockup with outputs high</t>
-  </si>
-  <si>
-    <t>Controller lockup with outputs low</t>
-  </si>
-  <si>
-    <t>Loss of magic smoke</t>
-  </si>
-  <si>
     <t>Software bug; Hardware failure</t>
   </si>
   <si>
-    <t>4.1.2</t>
-  </si>
-  <si>
-    <t>4.1.3</t>
-  </si>
-  <si>
     <t>MCU</t>
   </si>
   <si>
@@ -3379,15 +3358,6 @@
     <t>Chamber Heater Assy</t>
   </si>
   <si>
-    <t>Controls</t>
-  </si>
-  <si>
-    <t>Hotend</t>
-  </si>
-  <si>
-    <t>Hotend Assy</t>
-  </si>
-  <si>
     <t>3.1.1</t>
   </si>
   <si>
@@ -3466,27 +3436,9 @@
     <t>Heater sags down onto metal mounting plate</t>
   </si>
   <si>
-    <t>No heaters receive power</t>
-  </si>
-  <si>
-    <t>SW loops stops monitoring sensors; previous output state is indeterminate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thermal fuse on bed heater; Thermal fuse on bed SSR; Current fuse on bed SSR; Thermal fuse on chamber heater; Thermal fuse on chamber SSR; Current fuse on chamber SSR; </t>
-  </si>
-  <si>
     <t>Contactor outputs release; SSR switches off</t>
   </si>
   <si>
-    <t>Short circuit, Damage from reverse voltage spike on contactor release; Hardware failure</t>
-  </si>
-  <si>
-    <t>Heaters may continue to receive power</t>
-  </si>
-  <si>
-    <t>Power continues to flow to heaters</t>
-  </si>
-  <si>
     <t>Contactor outputs stay closed; SSRs switch on with 100% duty cycle</t>
   </si>
   <si>
@@ -3502,7 +3454,172 @@
     <t>Open circuit NTC thermistor wire</t>
   </si>
   <si>
-    <t>Software bug; Hardware failure / mosfet fused closed</t>
+    <t>1.5.1</t>
+  </si>
+  <si>
+    <t>1.6.1</t>
+  </si>
+  <si>
+    <t>RPi</t>
+  </si>
+  <si>
+    <t>1.5.2</t>
+  </si>
+  <si>
+    <t>Moonraker control loop + mains relay</t>
+  </si>
+  <si>
+    <t>Klipper/moonraker timeout on RPI</t>
+  </si>
+  <si>
+    <t>Mains relay opens</t>
+  </si>
+  <si>
+    <t>All power to printer is cut</t>
+  </si>
+  <si>
+    <t>Software bug; Hardware failure / mosfet fused closed; Damage from reverse voltage spike on contactor release</t>
+  </si>
+  <si>
+    <t>Controller failure with outputs high</t>
+  </si>
+  <si>
+    <t>Controller failure with outputs low</t>
+  </si>
+  <si>
+    <t>Controller failure/restart with GPIO low</t>
+  </si>
+  <si>
+    <t>1.6.2</t>
+  </si>
+  <si>
+    <t>Controller failure/restart with GPIO high</t>
+  </si>
+  <si>
+    <t>Mains relay stays closed; printer continues to operate</t>
+  </si>
+  <si>
+    <t>MCU times out</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Software bug; Damage from reverse voltage spike on relay coil release; Hardware failure</t>
+  </si>
+  <si>
+    <t>Software bug;  Damage from reverse voltage spike on relay coil release; Hardware failure</t>
+  </si>
+  <si>
+    <t>3.6.1</t>
+  </si>
+  <si>
+    <t>3.6.2</t>
+  </si>
+  <si>
+    <t>3.7.1</t>
+  </si>
+  <si>
+    <t>3.7.2</t>
+  </si>
+  <si>
+    <t>Heater does not receive power</t>
+  </si>
+  <si>
+    <t>2.1.2</t>
+  </si>
+  <si>
+    <t>Open circuit</t>
+  </si>
+  <si>
+    <t>2.1.3</t>
+  </si>
+  <si>
+    <t>Loose wire connection</t>
+  </si>
+  <si>
+    <t>Vibration; Exposure to high temperature on connector; Corrosion</t>
+  </si>
+  <si>
+    <t>Current fuse; Thermistor + SW control loop</t>
+  </si>
+  <si>
+    <t>Use of vibration and high temp rated connectors</t>
+  </si>
+  <si>
+    <t>Don't overspec heater wattage beyond what is needed for intended volumetric flow</t>
+  </si>
+  <si>
+    <t>Thermistor</t>
+  </si>
+  <si>
+    <t>1.1.7</t>
+  </si>
+  <si>
+    <t>Short circuit NTC thermistor wire</t>
+  </si>
+  <si>
+    <t>Thermistor resistance decreases to zero</t>
+  </si>
+  <si>
+    <t>2.2.1</t>
+  </si>
+  <si>
+    <t>2.2.2</t>
+  </si>
+  <si>
+    <t>Short circuit PTC thermistor wire</t>
+  </si>
+  <si>
+    <t>3.1.7</t>
+  </si>
+  <si>
+    <t>Vibration; Improper strain relief; Caught in motion system</t>
+  </si>
+  <si>
+    <t>Mechanical damage</t>
+  </si>
+  <si>
+    <t>2.3.1</t>
+  </si>
+  <si>
+    <t>Toolhead Assy</t>
+  </si>
+  <si>
+    <t>Toolhead</t>
+  </si>
+  <si>
+    <t>Switch off mosfet before switching off contactor &amp; vice versa to minimize spark</t>
+  </si>
+  <si>
+    <t>2.4.1</t>
+  </si>
+  <si>
+    <t>2.4.2</t>
+  </si>
+  <si>
+    <t>2.5.1</t>
+  </si>
+  <si>
+    <t>2.5.2</t>
+  </si>
+  <si>
+    <t>Contactor outputs stay closed; mosfets switch on with 100% duty cycle</t>
+  </si>
+  <si>
+    <t>Contactor outputs release; mosfet switches off</t>
+  </si>
+  <si>
+    <t>Current fuse on cartridge heater; Thermistor on heater + SW control loop; Klipper/moonraker timeout on RPI</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Software bug; Damage from reverse voltage spike on contactor coil release; Hardware failure</t>
+  </si>
+  <si>
+    <t>Software bug;  Damage from reverse voltage spike on contactor coil release; Hardware failure</t>
+  </si>
+  <si>
+    <t>Thermal fuse on chamber heater; Thermal fuse on chamber SSR; Current fuse on chamber SSR; Thermistor on heater + SW control loop; Klipper/moonraker timeout on RPI</t>
+  </si>
+  <si>
+    <t>Thermal fuse on bed heater; Thermal fuse on bed SSR; Current fuse on bed SSR; Thermistor on heater + SW control loop; Klipper/moonraker timeout on RPI</t>
   </si>
 </sst>
 </file>
@@ -4013,10 +4130,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20939D60-F13B-4603-AAC1-1CA252B6FC6A}">
-  <dimension ref="A1:P72"/>
+  <dimension ref="A1:P83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4112,7 +4229,7 @@
     </row>
     <row r="3" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
-        <v>1115</v>
+        <v>1108</v>
       </c>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
@@ -4211,7 +4328,7 @@
         <v>1035</v>
       </c>
       <c r="J5" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K5" s="4" t="s">
         <v>1054</v>
@@ -4221,7 +4338,7 @@
       </c>
       <c r="M5" s="4">
         <f>H5*J5*L5</f>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="N5" s="4" t="s">
         <v>1054</v>
@@ -4245,7 +4362,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>1157</v>
+        <v>1141</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>1055</v>
@@ -4263,7 +4380,7 @@
         <v>1035</v>
       </c>
       <c r="J6" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>1056</v>
@@ -4272,8 +4389,8 @@
         <v>2</v>
       </c>
       <c r="M6" s="4">
-        <f t="shared" ref="M6:M33" si="0">H6*J6*L6</f>
-        <v>12</v>
+        <f t="shared" ref="M6:M48" si="0">H6*J6*L6</f>
+        <v>24</v>
       </c>
       <c r="N6" s="4" t="s">
         <v>1056</v>
@@ -4286,7 +4403,7 @@
         <v>L</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>1034</v>
       </c>
@@ -4297,45 +4414,45 @@
         <v>5</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>1058</v>
+        <v>1175</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>1059</v>
+        <v>1176</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>1060</v>
+        <v>1139</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>1027</v>
       </c>
       <c r="H7" s="4">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>1061</v>
+        <v>1035</v>
       </c>
       <c r="J7" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>1062</v>
+        <v>1056</v>
       </c>
       <c r="L7" s="4">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="M7" s="4">
         <f t="shared" si="0"/>
-        <v>147</v>
+        <v>2</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>1064</v>
+        <v>1056</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>1063</v>
+        <v>12</v>
       </c>
       <c r="P7" s="4" t="str">
         <f>VLOOKUP((H7&amp;J7&amp;L7),AP_lookup_table!D5:E1004,2,FALSE)</f>
-        <v>M</v>
+        <v>L</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4349,48 +4466,48 @@
         <v>5</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>1066</v>
+        <v>1058</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>1067</v>
+        <v>1059</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>1068</v>
+        <v>1060</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>1027</v>
       </c>
       <c r="H8" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>1069</v>
+        <v>1061</v>
       </c>
       <c r="J8" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>1070</v>
+        <v>1062</v>
       </c>
       <c r="L8" s="4">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="M8" s="4">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>147</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>1075</v>
+        <v>1064</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>1071</v>
+        <v>1063</v>
       </c>
       <c r="P8" s="4" t="str">
-        <f>VLOOKUP((H8&amp;J8&amp;L8),AP_lookup_table!D6:E1005,2,FALSE)</f>
-        <v>L</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <f>VLOOKUP((H8&amp;J8&amp;L8),AP_lookup_table!D5:E1004,2,FALSE)</f>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>1043</v>
       </c>
@@ -4401,41 +4518,41 @@
         <v>5</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>1047</v>
+        <v>1066</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>1072</v>
+        <v>1067</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>1081</v>
+        <v>1068</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>1074</v>
+        <v>1027</v>
       </c>
       <c r="H9" s="4">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>1088</v>
+        <v>1169</v>
       </c>
       <c r="J9" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>1062</v>
+        <v>1070</v>
       </c>
       <c r="L9" s="4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M9" s="4">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>1076</v>
+        <v>1171</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>1077</v>
+        <v>1071</v>
       </c>
       <c r="P9" s="4" t="str">
         <f>VLOOKUP((H9&amp;J9&amp;L9),AP_lookup_table!D6:E1005,2,FALSE)</f>
@@ -4444,111 +4561,111 @@
     </row>
     <row r="10" spans="1:16" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>1036</v>
+        <v>1174</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>1030</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>1037</v>
+        <v>5</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>1038</v>
+        <v>1047</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>1087</v>
+        <v>1072</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>1060</v>
+        <v>1081</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>1027</v>
+        <v>1074</v>
       </c>
       <c r="H10" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>1035</v>
+        <v>1088</v>
       </c>
       <c r="J10" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K10" s="4" t="s">
         <v>1062</v>
       </c>
       <c r="L10" s="4">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="M10" s="4">
         <f t="shared" si="0"/>
-        <v>98</v>
+        <v>40</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>12</v>
+        <v>1076</v>
       </c>
       <c r="O10" s="4" t="s">
-        <v>1143</v>
+        <v>1077</v>
       </c>
       <c r="P10" s="4" t="str">
-        <f>VLOOKUP((H10&amp;J10&amp;L10),AP_lookup_table!D7:E1006,2,FALSE)</f>
-        <v>M</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="66.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <f>VLOOKUP((H10&amp;J10&amp;L10),AP_lookup_table!D6:E1005,2,FALSE)</f>
+        <v>L</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>1044</v>
+        <v>1036</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>1030</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>1040</v>
+        <v>1037</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>1094</v>
+        <v>1038</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>1078</v>
+        <v>1087</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>1079</v>
+        <v>1060</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>3</v>
+        <v>1027</v>
       </c>
       <c r="H11" s="4">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>1089</v>
+        <v>1035</v>
       </c>
       <c r="J11" s="4">
         <v>2</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>1080</v>
+        <v>1062</v>
       </c>
       <c r="L11" s="4">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="M11" s="4">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>98</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>1080</v>
+        <v>12</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>12</v>
+        <v>1133</v>
       </c>
       <c r="P11" s="4" t="str">
         <f>VLOOKUP((H11&amp;J11&amp;L11),AP_lookup_table!D7:E1006,2,FALSE)</f>
-        <v>L</v>
+        <v>M</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="66.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>1030</v>
@@ -4557,50 +4674,50 @@
         <v>1040</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>1090</v>
+        <v>1078</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>1091</v>
+        <v>1079</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>1027</v>
+        <v>3</v>
       </c>
       <c r="H12" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>1092</v>
+        <v>1089</v>
       </c>
       <c r="J12" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>1096</v>
+        <v>1080</v>
       </c>
       <c r="L12" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M12" s="4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>1093</v>
+        <v>1080</v>
       </c>
       <c r="O12" s="4" t="s">
         <v>12</v>
       </c>
       <c r="P12" s="4" t="str">
-        <f>VLOOKUP((H12&amp;J12&amp;L12),AP_lookup_table!D8:E1007,2,FALSE)</f>
+        <f>VLOOKUP((H12&amp;J12&amp;L12),AP_lookup_table!D7:E1006,2,FALSE)</f>
         <v>L</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" ht="66.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>1086</v>
+        <v>1045</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>1030</v>
@@ -4609,38 +4726,38 @@
         <v>1040</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>1048</v>
+        <v>1095</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>1049</v>
+        <v>1090</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>1084</v>
+        <v>1091</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>3</v>
+        <v>1027</v>
       </c>
       <c r="H13" s="4">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>1082</v>
+        <v>1092</v>
       </c>
       <c r="J13" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>1083</v>
+        <v>1096</v>
       </c>
       <c r="L13" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M13" s="4">
         <f t="shared" si="0"/>
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>1085</v>
+        <v>1093</v>
       </c>
       <c r="O13" s="4" t="s">
         <v>12</v>
@@ -4650,614 +4767,664 @@
         <v>L</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>1046</v>
+        <v>1086</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>1030</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>1094</v>
+        <v>1048</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>1100</v>
+        <v>1049</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>1098</v>
+        <v>1084</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>1099</v>
+        <v>3</v>
       </c>
       <c r="H14" s="4">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>1101</v>
+        <v>1082</v>
       </c>
       <c r="J14" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>1062</v>
+        <v>1083</v>
       </c>
       <c r="L14" s="4">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="M14" s="4">
         <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>1085</v>
+      </c>
+      <c r="O14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="P14" s="4" t="str">
+        <f>VLOOKUP((H14&amp;J14&amp;L14),AP_lookup_table!D8:E1007,2,FALSE)</f>
+        <v>L</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>1030</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>1094</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>1100</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>1098</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>1099</v>
+      </c>
+      <c r="H15" s="4">
+        <v>6</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>1101</v>
+      </c>
+      <c r="J15" s="4">
+        <v>1</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>1062</v>
+      </c>
+      <c r="L15" s="4">
+        <v>7</v>
+      </c>
+      <c r="M15" s="4">
+        <f>H15*J15*L15</f>
         <v>42</v>
       </c>
-      <c r="N14" s="4" t="s">
+      <c r="N15" s="4" t="s">
         <v>1102</v>
       </c>
-      <c r="O14" s="4" t="s">
+      <c r="O15" s="4" t="s">
         <v>1102</v>
       </c>
-      <c r="P14" s="4" t="str">
-        <f>VLOOKUP((H14&amp;J14&amp;L14),AP_lookup_table!D11:E1010,2,FALSE)</f>
+      <c r="P15" s="4" t="str">
+        <f>VLOOKUP((H15&amp;J15&amp;L15),AP_lookup_table!D11:E1010,2,FALSE)</f>
         <v>L</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="11" t="s">
-        <v>1119</v>
-      </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="12"/>
-      <c r="N15" s="12"/>
-      <c r="O15" s="12"/>
-      <c r="P15" s="13"/>
-    </row>
-    <row r="16" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" ht="109.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>1112</v>
+        <v>1142</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>1118</v>
+        <v>1030</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>1131</v>
-      </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
+        <v>1104</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>1151</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>1137</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>1079</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H16" s="4">
+        <v>10</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>1150</v>
+      </c>
+      <c r="J16" s="4">
+        <v>2</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>1197</v>
+      </c>
+      <c r="L16" s="4">
+        <v>1</v>
+      </c>
       <c r="M16" s="4">
-        <f t="shared" ref="M16" si="1">H16*J16*L16</f>
-        <v>0</v>
-      </c>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
-      <c r="P16" s="4" t="e">
-        <f>VLOOKUP((H16&amp;J16&amp;L16),AP_lookup_table!D16:E1015,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="11" t="s">
-        <v>1116</v>
-      </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="12"/>
-      <c r="O17" s="12"/>
-      <c r="P17" s="13"/>
-    </row>
-    <row r="18" spans="1:16" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" ref="M16:M19" si="1">H16*J16*L16</f>
+        <v>20</v>
+      </c>
+      <c r="N16" s="4" t="s">
+        <v>1146</v>
+      </c>
+      <c r="O16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="P16" s="4" t="str">
+        <f>VLOOKUP((H16&amp;J16&amp;L16),AP_lookup_table!D12:E1011,2,FALSE)</f>
+        <v>L</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>1030</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>1104</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>1152</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>1136</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>1164</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>1027</v>
+      </c>
+      <c r="H17" s="4">
+        <v>1</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>1103</v>
+      </c>
+      <c r="J17" s="4">
+        <v>1</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>1147</v>
+      </c>
+      <c r="L17" s="4">
+        <v>3</v>
+      </c>
+      <c r="M17" s="4">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="N17" s="4" t="s">
+        <v>1146</v>
+      </c>
+      <c r="O17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="P17" s="4" t="str">
+        <f>VLOOKUP((H17&amp;J17&amp;L17),AP_lookup_table!D13:E1012,2,FALSE)</f>
+        <v>L</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>1120</v>
+        <v>1143</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>1113</v>
+        <v>1030</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>1114</v>
+        <v>1144</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>1028</v>
+        <v>1155</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>14</v>
+        <v>1156</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>13</v>
+        <v>1157</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>3</v>
+        <v>1027</v>
       </c>
       <c r="H18" s="4">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>1065</v>
+        <v>1158</v>
       </c>
       <c r="J18" s="4">
         <v>1</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>1042</v>
+        <v>1062</v>
       </c>
       <c r="L18" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M18" s="4">
-        <f>H18*J18*L18</f>
-        <v>20</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="N18" s="4" t="s">
-        <v>1042</v>
+        <v>12</v>
       </c>
       <c r="O18" s="4" t="s">
         <v>12</v>
       </c>
       <c r="P18" s="4" t="str">
-        <f>VLOOKUP((H18&amp;J18&amp;L18),AP_lookup_table!D13:E1012,2,FALSE)</f>
+        <f>VLOOKUP((H18&amp;J18&amp;L18),AP_lookup_table!D14:E1013,2,FALSE)</f>
         <v>L</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>1121</v>
+        <v>1154</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>1113</v>
+        <v>1030</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>1114</v>
+        <v>1144</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>1051</v>
+        <v>1153</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>1052</v>
+        <v>1148</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>1053</v>
+        <v>1149</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>1027</v>
       </c>
       <c r="H19" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>1035</v>
+        <v>1159</v>
       </c>
       <c r="J19" s="4">
         <v>2</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>1054</v>
+        <v>1062</v>
       </c>
       <c r="L19" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M19" s="4">
-        <f>H19*J19*L19</f>
-        <v>8</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="N19" s="4" t="s">
-        <v>1054</v>
+        <v>12</v>
       </c>
       <c r="O19" s="4" t="s">
         <v>12</v>
       </c>
       <c r="P19" s="4" t="str">
-        <f>VLOOKUP((H19&amp;J19&amp;L19),AP_lookup_table!D14:E1013,2,FALSE)</f>
+        <f>VLOOKUP((H19&amp;J19&amp;L19),AP_lookup_table!D15:E1014,2,FALSE)</f>
         <v>L</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
-        <v>1122</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>1113</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>1114</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>1156</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>1055</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>1155</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>1027</v>
-      </c>
-      <c r="H20" s="4">
-        <v>3</v>
-      </c>
-      <c r="I20" s="4" t="s">
-        <v>1035</v>
-      </c>
-      <c r="J20" s="4">
-        <v>2</v>
-      </c>
-      <c r="K20" s="4" t="s">
-        <v>1056</v>
-      </c>
-      <c r="L20" s="4">
-        <v>2</v>
-      </c>
-      <c r="M20" s="4">
-        <f t="shared" ref="M20:M28" si="2">H20*J20*L20</f>
-        <v>12</v>
-      </c>
-      <c r="N20" s="4" t="s">
-        <v>1056</v>
-      </c>
-      <c r="O20" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="P20" s="4" t="str">
-        <f>VLOOKUP((H20&amp;J20&amp;L20),AP_lookup_table!D15:E1014,2,FALSE)</f>
+    <row r="20" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="11" t="s">
+        <v>1184</v>
+      </c>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="12"/>
+      <c r="P20" s="13"/>
+    </row>
+    <row r="21" spans="1:16" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>1105</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>1121</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H21" s="4">
+        <v>10</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>1065</v>
+      </c>
+      <c r="J21" s="4">
+        <v>2</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>1170</v>
+      </c>
+      <c r="L21" s="4">
+        <v>4</v>
+      </c>
+      <c r="M21" s="4">
+        <f t="shared" ref="M21:M30" si="2">H21*J21*L21</f>
+        <v>80</v>
+      </c>
+      <c r="N21" s="4" t="s">
+        <v>1054</v>
+      </c>
+      <c r="O21" s="4" t="s">
+        <v>1172</v>
+      </c>
+      <c r="P21" s="4" t="str">
+        <f>VLOOKUP((H21&amp;J21&amp;L21),AP_lookup_table!D17:E1016,2,FALSE)</f>
         <v>L</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
-        <v>1123</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>1113</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>1114</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>1058</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>1059</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>1060</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>1027</v>
-      </c>
-      <c r="H21" s="4">
-        <v>7</v>
-      </c>
-      <c r="I21" s="4" t="s">
-        <v>1061</v>
-      </c>
-      <c r="J21" s="4">
-        <v>3</v>
-      </c>
-      <c r="K21" s="4" t="s">
-        <v>1062</v>
-      </c>
-      <c r="L21" s="4">
-        <v>7</v>
-      </c>
-      <c r="M21" s="4">
-        <f t="shared" si="2"/>
-        <v>147</v>
-      </c>
-      <c r="N21" s="4" t="s">
-        <v>1064</v>
-      </c>
-      <c r="O21" s="4" t="s">
-        <v>1063</v>
-      </c>
-      <c r="P21" s="4" t="str">
-        <f>VLOOKUP((H21&amp;J21&amp;L21),AP_lookup_table!D16:E1015,2,FALSE)</f>
-        <v>M</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>1124</v>
+        <v>1165</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>1113</v>
+        <v>1185</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>1114</v>
+        <v>1121</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>1066</v>
+        <v>1166</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>1067</v>
+        <v>1052</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>1068</v>
+        <v>1053</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>1027</v>
       </c>
       <c r="H22" s="4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>1069</v>
+        <v>1035</v>
       </c>
       <c r="J22" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>1070</v>
+        <v>1054</v>
       </c>
       <c r="L22" s="4">
         <v>3</v>
       </c>
       <c r="M22" s="4">
         <f t="shared" si="2"/>
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="N22" s="4" t="s">
-        <v>1075</v>
+        <v>1054</v>
       </c>
       <c r="O22" s="4" t="s">
-        <v>1071</v>
+        <v>1063</v>
       </c>
       <c r="P22" s="4" t="str">
-        <f>VLOOKUP((H22&amp;J22&amp;L22),AP_lookup_table!D17:E1016,2,FALSE)</f>
+        <f>VLOOKUP((H22&amp;J22&amp;L22),AP_lookup_table!D18:E1017,2,FALSE)</f>
         <v>L</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>1125</v>
+        <v>1167</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>1113</v>
+        <v>1185</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>1114</v>
+        <v>1121</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>1144</v>
+        <v>1168</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>1145</v>
+        <v>1067</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>1027</v>
+        <v>1068</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>1027</v>
       </c>
       <c r="H23" s="4">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>1141</v>
+        <v>1169</v>
       </c>
       <c r="J23" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>1062</v>
+        <v>1070</v>
       </c>
       <c r="L23" s="4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M23" s="4">
         <f t="shared" si="2"/>
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="N23" s="4" t="s">
-        <v>12</v>
+        <v>1171</v>
       </c>
       <c r="O23" s="4" t="s">
-        <v>1142</v>
+        <v>1071</v>
       </c>
       <c r="P23" s="4" t="str">
-        <f>VLOOKUP((H23&amp;J23&amp;L23),AP_lookup_table!D17:E1016,2,FALSE)</f>
+        <f>VLOOKUP((H23&amp;J23&amp;L23),AP_lookup_table!D19:E1018,2,FALSE)</f>
         <v>L</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>1126</v>
+        <v>1177</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>1113</v>
+        <v>1185</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>1154</v>
+        <v>1173</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>1038</v>
+        <v>1179</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>1087</v>
+        <v>1176</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>1060</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>1027</v>
-      </c>
+        <v>1073</v>
+      </c>
+      <c r="G24" s="4"/>
       <c r="H24" s="4">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I24" s="4" t="s">
         <v>1035</v>
       </c>
       <c r="J24" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>1062</v>
+        <v>1056</v>
       </c>
       <c r="L24" s="4">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="M24" s="4">
         <f t="shared" si="2"/>
-        <v>98</v>
+        <v>6</v>
       </c>
       <c r="N24" s="4" t="s">
+        <v>1056</v>
+      </c>
+      <c r="O24" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="O24" s="4" t="s">
-        <v>1143</v>
-      </c>
       <c r="P24" s="4" t="str">
-        <f>VLOOKUP((H24&amp;J24&amp;L24),AP_lookup_table!D18:E1017,2,FALSE)</f>
-        <v>M</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" ht="66.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <f>VLOOKUP((H24&amp;J24&amp;L24),AP_lookup_table!D20:E1019,2,FALSE)</f>
+        <v>L</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>1127</v>
+        <v>1178</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>1113</v>
+        <v>1185</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>1040</v>
+        <v>1173</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>1094</v>
+        <v>1140</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>1078</v>
+        <v>1055</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>1079</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>3</v>
-      </c>
+        <v>1139</v>
+      </c>
+      <c r="G25" s="4"/>
       <c r="H25" s="4">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>1089</v>
+        <v>1035</v>
       </c>
       <c r="J25" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>1080</v>
+        <v>1056</v>
       </c>
       <c r="L25" s="4">
         <v>2</v>
       </c>
       <c r="M25" s="4">
         <f t="shared" si="2"/>
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="N25" s="4" t="s">
-        <v>1080</v>
+        <v>1056</v>
       </c>
       <c r="O25" s="4" t="s">
         <v>12</v>
       </c>
       <c r="P25" s="4" t="str">
-        <f>VLOOKUP((H25&amp;J25&amp;L25),AP_lookup_table!D18:E1017,2,FALSE)</f>
+        <f>VLOOKUP((H25&amp;J25&amp;L25),AP_lookup_table!D21:E1020,2,FALSE)</f>
         <v>L</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="66.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>1128</v>
+        <v>1183</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>1113</v>
+        <v>1185</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>1040</v>
+        <v>1041</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>1090</v>
+        <v>1100</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>1091</v>
+        <v>1098</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>1027</v>
+        <v>1099</v>
       </c>
       <c r="H26" s="4">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>1092</v>
+        <v>1101</v>
       </c>
       <c r="J26" s="4">
         <v>1</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>1096</v>
+        <v>1062</v>
       </c>
       <c r="L26" s="4">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="M26" s="4">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="N26" s="4" t="s">
-        <v>1093</v>
+        <v>1186</v>
       </c>
       <c r="O26" s="4" t="s">
-        <v>12</v>
+        <v>1186</v>
       </c>
       <c r="P26" s="4" t="str">
-        <f>VLOOKUP((H26&amp;J26&amp;L26),AP_lookup_table!D19:E1018,2,FALSE)</f>
+        <f>VLOOKUP((H26&amp;J26&amp;L26),AP_lookup_table!D22:E1021,2,FALSE)</f>
         <v>L</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>1129</v>
+        <v>1187</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>1113</v>
+        <v>1185</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>1040</v>
+        <v>1104</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>1048</v>
+        <v>1151</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>1049</v>
+        <v>1191</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>1084</v>
+        <v>1079</v>
       </c>
       <c r="G27" s="4" t="s">
         <v>3</v>
@@ -5266,581 +5433,1091 @@
         <v>10</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>1082</v>
+        <v>1150</v>
       </c>
       <c r="J27" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>1083</v>
+        <v>1193</v>
       </c>
       <c r="L27" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M27" s="4">
         <f t="shared" si="2"/>
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="N27" s="4" t="s">
-        <v>1085</v>
+        <v>1146</v>
       </c>
       <c r="O27" s="4" t="s">
         <v>12</v>
       </c>
       <c r="P27" s="4" t="str">
-        <f>VLOOKUP((H27&amp;J27&amp;L27),AP_lookup_table!D19:E1018,2,FALSE)</f>
+        <f>VLOOKUP((H27&amp;J27&amp;L27),AP_lookup_table!D13:E1012,2,FALSE)</f>
         <v>L</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>1130</v>
+        <v>1188</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>1113</v>
+        <v>1185</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>1041</v>
+        <v>1104</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>1094</v>
+        <v>1152</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>1100</v>
+        <v>1192</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>1098</v>
+        <v>1164</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>1099</v>
+        <v>1027</v>
       </c>
       <c r="H28" s="4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>1101</v>
+        <v>1103</v>
       </c>
       <c r="J28" s="4">
         <v>1</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>1062</v>
+        <v>1147</v>
       </c>
       <c r="L28" s="4">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="M28" s="4">
         <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="N28" s="4" t="s">
+        <v>1146</v>
+      </c>
+      <c r="O28" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="P28" s="4" t="str">
+        <f>VLOOKUP((H28&amp;J28&amp;L28),AP_lookup_table!D14:E1013,2,FALSE)</f>
+        <v>L</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>1189</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>1144</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>1155</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>1156</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>1157</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>1027</v>
+      </c>
+      <c r="H29" s="4">
+        <v>1</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>1194</v>
+      </c>
+      <c r="J29" s="4">
+        <v>1</v>
+      </c>
+      <c r="K29" s="4" t="s">
+        <v>1062</v>
+      </c>
+      <c r="L29" s="4">
+        <v>1</v>
+      </c>
+      <c r="M29" s="4">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="N29" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="O29" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="P29" s="4" t="str">
+        <f>VLOOKUP((H29&amp;J29&amp;L29),AP_lookup_table!D15:E1014,2,FALSE)</f>
+        <v>L</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
+        <v>1190</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>1144</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>1153</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>1148</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>1149</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>1027</v>
+      </c>
+      <c r="H30" s="4">
+        <v>1</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>1195</v>
+      </c>
+      <c r="J30" s="4">
+        <v>2</v>
+      </c>
+      <c r="K30" s="4" t="s">
+        <v>1062</v>
+      </c>
+      <c r="L30" s="4">
+        <v>1</v>
+      </c>
+      <c r="M30" s="4">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="N30" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="O30" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="P30" s="4" t="str">
+        <f>VLOOKUP((H30&amp;J30&amp;L30),AP_lookup_table!D16:E1015,2,FALSE)</f>
+        <v>L</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="11" t="s">
+        <v>1109</v>
+      </c>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="12"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="12"/>
+      <c r="M31" s="12"/>
+      <c r="N31" s="12"/>
+      <c r="O31" s="12"/>
+      <c r="P31" s="13"/>
+    </row>
+    <row r="32" spans="1:16" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
+        <v>1110</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H32" s="4">
+        <v>10</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>1065</v>
+      </c>
+      <c r="J32" s="4">
+        <v>1</v>
+      </c>
+      <c r="K32" s="4" t="s">
+        <v>1042</v>
+      </c>
+      <c r="L32" s="4">
+        <v>2</v>
+      </c>
+      <c r="M32" s="4">
+        <f>H32*J32*L32</f>
+        <v>20</v>
+      </c>
+      <c r="N32" s="4" t="s">
+        <v>1042</v>
+      </c>
+      <c r="O32" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="P32" s="4" t="str">
+        <f>VLOOKUP((H32&amp;J32&amp;L32),AP_lookup_table!D13:E1012,2,FALSE)</f>
+        <v>L</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
+        <v>1111</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>1051</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>1052</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>1053</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>1027</v>
+      </c>
+      <c r="H33" s="4">
+        <v>2</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>1181</v>
+      </c>
+      <c r="J33" s="4">
+        <v>2</v>
+      </c>
+      <c r="K33" s="4" t="s">
+        <v>1054</v>
+      </c>
+      <c r="L33" s="4">
+        <v>2</v>
+      </c>
+      <c r="M33" s="4">
+        <f>H33*J33*L33</f>
+        <v>8</v>
+      </c>
+      <c r="N33" s="4" t="s">
+        <v>1054</v>
+      </c>
+      <c r="O33" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="P33" s="4" t="str">
+        <f>VLOOKUP((H33&amp;J33&amp;L33),AP_lookup_table!D14:E1013,2,FALSE)</f>
+        <v>L</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
+        <v>1112</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>1140</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>1055</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>1139</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>1027</v>
+      </c>
+      <c r="H34" s="4">
+        <v>1</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>1181</v>
+      </c>
+      <c r="J34" s="4">
+        <v>4</v>
+      </c>
+      <c r="K34" s="4" t="s">
+        <v>1056</v>
+      </c>
+      <c r="L34" s="4">
+        <v>2</v>
+      </c>
+      <c r="M34" s="4">
+        <f t="shared" ref="M34:M43" si="3">H34*J34*L34</f>
+        <v>8</v>
+      </c>
+      <c r="N34" s="4" t="s">
+        <v>1056</v>
+      </c>
+      <c r="O34" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="P34" s="4" t="str">
+        <f>VLOOKUP((H34&amp;J34&amp;L34),AP_lookup_table!D15:E1014,2,FALSE)</f>
+        <v>L</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
+        <v>1113</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>1179</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>1176</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>1073</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>1027</v>
+      </c>
+      <c r="H35" s="4">
+        <v>3</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>1181</v>
+      </c>
+      <c r="J35" s="4">
+        <v>1</v>
+      </c>
+      <c r="K35" s="4" t="s">
+        <v>1056</v>
+      </c>
+      <c r="L35" s="4">
+        <v>2</v>
+      </c>
+      <c r="M35" s="4">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="N35" s="4" t="s">
+        <v>1056</v>
+      </c>
+      <c r="O35" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="P35" s="4" t="str">
+        <f>VLOOKUP((H35&amp;J35&amp;L35),AP_lookup_table!D16:E1015,2,FALSE)</f>
+        <v>L</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
+        <v>1114</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>1058</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>1059</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>1060</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>1027</v>
+      </c>
+      <c r="H36" s="4">
+        <v>7</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>1182</v>
+      </c>
+      <c r="J36" s="4">
+        <v>3</v>
+      </c>
+      <c r="K36" s="4" t="s">
+        <v>1062</v>
+      </c>
+      <c r="L36" s="4">
+        <v>7</v>
+      </c>
+      <c r="M36" s="4">
+        <f t="shared" si="3"/>
+        <v>147</v>
+      </c>
+      <c r="N36" s="4" t="s">
+        <v>1064</v>
+      </c>
+      <c r="O36" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="P36" s="4" t="str">
+        <f>VLOOKUP((H36&amp;J36&amp;L36),AP_lookup_table!D16:E1015,2,FALSE)</f>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
+        <v>1115</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>1066</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>1067</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>1068</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>1027</v>
+      </c>
+      <c r="H37" s="4">
+        <v>6</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>1069</v>
+      </c>
+      <c r="J37" s="4">
+        <v>2</v>
+      </c>
+      <c r="K37" s="4" t="s">
+        <v>1070</v>
+      </c>
+      <c r="L37" s="4">
+        <v>3</v>
+      </c>
+      <c r="M37" s="4">
+        <f t="shared" si="3"/>
+        <v>36</v>
+      </c>
+      <c r="N37" s="4" t="s">
+        <v>1075</v>
+      </c>
+      <c r="O37" s="4" t="s">
+        <v>1071</v>
+      </c>
+      <c r="P37" s="4" t="str">
+        <f>VLOOKUP((H37&amp;J37&amp;L37),AP_lookup_table!D17:E1016,2,FALSE)</f>
+        <v>L</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
+        <v>1180</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>1135</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>1027</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>1027</v>
+      </c>
+      <c r="H38" s="4">
+        <v>4</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>1131</v>
+      </c>
+      <c r="J38" s="4">
+        <v>2</v>
+      </c>
+      <c r="K38" s="4" t="s">
+        <v>1062</v>
+      </c>
+      <c r="L38" s="4">
+        <v>5</v>
+      </c>
+      <c r="M38" s="4">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="N38" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="O38" s="4" t="s">
+        <v>1132</v>
+      </c>
+      <c r="P38" s="4" t="str">
+        <f>VLOOKUP((H38&amp;J38&amp;L38),AP_lookup_table!D17:E1016,2,FALSE)</f>
+        <v>L</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>1138</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>1038</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>1060</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>1027</v>
+      </c>
+      <c r="H39" s="4">
+        <v>7</v>
+      </c>
+      <c r="I39" s="4" t="s">
+        <v>1181</v>
+      </c>
+      <c r="J39" s="4">
+        <v>2</v>
+      </c>
+      <c r="K39" s="4" t="s">
+        <v>1062</v>
+      </c>
+      <c r="L39" s="4">
+        <v>7</v>
+      </c>
+      <c r="M39" s="4">
+        <f t="shared" si="3"/>
+        <v>98</v>
+      </c>
+      <c r="N39" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="O39" s="4" t="s">
+        <v>1133</v>
+      </c>
+      <c r="P39" s="4" t="str">
+        <f>VLOOKUP((H39&amp;J39&amp;L39),AP_lookup_table!D18:E1017,2,FALSE)</f>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" ht="66.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
+        <v>1117</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>1040</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>1094</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>1078</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>1079</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H40" s="4">
+        <v>10</v>
+      </c>
+      <c r="I40" s="4" t="s">
+        <v>1089</v>
+      </c>
+      <c r="J40" s="4">
+        <v>2</v>
+      </c>
+      <c r="K40" s="4" t="s">
+        <v>1080</v>
+      </c>
+      <c r="L40" s="4">
+        <v>2</v>
+      </c>
+      <c r="M40" s="4">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="N40" s="4" t="s">
+        <v>1080</v>
+      </c>
+      <c r="O40" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="P40" s="4" t="str">
+        <f>VLOOKUP((H40&amp;J40&amp;L40),AP_lookup_table!D18:E1017,2,FALSE)</f>
+        <v>L</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" ht="66.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
+        <v>1118</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>1040</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>1095</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>1090</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>1091</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>1027</v>
+      </c>
+      <c r="H41" s="4">
+        <v>1</v>
+      </c>
+      <c r="I41" s="4" t="s">
+        <v>1092</v>
+      </c>
+      <c r="J41" s="4">
+        <v>1</v>
+      </c>
+      <c r="K41" s="4" t="s">
+        <v>1096</v>
+      </c>
+      <c r="L41" s="4">
+        <v>1</v>
+      </c>
+      <c r="M41" s="4">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="N41" s="4" t="s">
+        <v>1093</v>
+      </c>
+      <c r="O41" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="P41" s="4" t="str">
+        <f>VLOOKUP((H41&amp;J41&amp;L41),AP_lookup_table!D19:E1018,2,FALSE)</f>
+        <v>L</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
+        <v>1119</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>1040</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>1048</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>1049</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>1084</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H42" s="4">
+        <v>10</v>
+      </c>
+      <c r="I42" s="4" t="s">
+        <v>1082</v>
+      </c>
+      <c r="J42" s="4">
+        <v>3</v>
+      </c>
+      <c r="K42" s="4" t="s">
+        <v>1083</v>
+      </c>
+      <c r="L42" s="4">
+        <v>2</v>
+      </c>
+      <c r="M42" s="4">
+        <f t="shared" si="3"/>
+        <v>60</v>
+      </c>
+      <c r="N42" s="4" t="s">
+        <v>1085</v>
+      </c>
+      <c r="O42" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="P42" s="4" t="str">
+        <f>VLOOKUP((H42&amp;J42&amp;L42),AP_lookup_table!D19:E1018,2,FALSE)</f>
+        <v>L</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
+        <v>1120</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>1094</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>1100</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>1098</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>1099</v>
+      </c>
+      <c r="H43" s="4">
+        <v>6</v>
+      </c>
+      <c r="I43" s="4" t="s">
+        <v>1101</v>
+      </c>
+      <c r="J43" s="4">
+        <v>1</v>
+      </c>
+      <c r="K43" s="4" t="s">
+        <v>1062</v>
+      </c>
+      <c r="L43" s="4">
+        <v>7</v>
+      </c>
+      <c r="M43" s="4">
+        <f t="shared" si="3"/>
         <v>42</v>
       </c>
-      <c r="N28" s="4" t="s">
+      <c r="N43" s="4" t="s">
         <v>1102</v>
       </c>
-      <c r="O28" s="4" t="s">
+      <c r="O43" s="4" t="s">
         <v>1102</v>
       </c>
-      <c r="P28" s="4" t="str">
-        <f>VLOOKUP((H28&amp;J28&amp;L28),AP_lookup_table!D22:E1021,2,FALSE)</f>
+      <c r="P43" s="4" t="str">
+        <f>VLOOKUP((H43&amp;J43&amp;L43),AP_lookup_table!D22:E1021,2,FALSE)</f>
         <v>L</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
-        <v>1132</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>1113</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>1133</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>1135</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>1138</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>1139</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>1140</v>
-      </c>
-      <c r="H29" s="4">
-        <v>5</v>
-      </c>
-      <c r="I29" s="4" t="s">
-        <v>1136</v>
-      </c>
-      <c r="J29" s="4">
-        <v>3</v>
-      </c>
-      <c r="K29" s="4" t="s">
-        <v>1134</v>
-      </c>
-      <c r="L29" s="4">
-        <v>2</v>
-      </c>
-      <c r="M29" s="4">
+    <row r="44" spans="1:16" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="4" t="s">
+        <v>1122</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>1123</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>1125</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>1128</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>1129</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>1130</v>
+      </c>
+      <c r="H44" s="4">
+        <v>5</v>
+      </c>
+      <c r="I44" s="4" t="s">
+        <v>1126</v>
+      </c>
+      <c r="J44" s="4">
+        <v>3</v>
+      </c>
+      <c r="K44" s="4" t="s">
+        <v>1124</v>
+      </c>
+      <c r="L44" s="4">
+        <v>2</v>
+      </c>
+      <c r="M44" s="4">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="N29" s="4" t="s">
+      <c r="N44" s="4" t="s">
+        <v>1127</v>
+      </c>
+      <c r="O44" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="P44" s="4" t="str">
+        <f>VLOOKUP((H44&amp;J44&amp;L44),AP_lookup_table!D12:E1011,2,FALSE)</f>
+        <v>L</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="4" t="s">
+        <v>1160</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>1104</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>1151</v>
+      </c>
+      <c r="E45" s="4" t="s">
         <v>1137</v>
       </c>
-      <c r="O29" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="P29" s="4" t="str">
-        <f>VLOOKUP((H29&amp;J29&amp;L29),AP_lookup_table!D12:E1011,2,FALSE)</f>
-        <v>L</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="11" t="s">
-        <v>1117</v>
-      </c>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
-      <c r="I30" s="12"/>
-      <c r="J30" s="12"/>
-      <c r="K30" s="12"/>
-      <c r="L30" s="12"/>
-      <c r="M30" s="12"/>
-      <c r="N30" s="12"/>
-      <c r="O30" s="12"/>
-      <c r="P30" s="13"/>
-    </row>
-    <row r="31" spans="1:16" ht="111" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="4" t="s">
-        <v>1103</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>1104</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>1111</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>1105</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>1153</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>1152</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H31" s="4">
-        <v>10</v>
-      </c>
-      <c r="I31" s="4" t="s">
-        <v>1158</v>
-      </c>
-      <c r="J31" s="4">
-        <v>2</v>
-      </c>
-      <c r="K31" s="4" t="s">
-        <v>1148</v>
-      </c>
-      <c r="L31" s="4">
-        <v>1</v>
-      </c>
-      <c r="M31" s="4">
+      <c r="F45" s="4" t="s">
+        <v>1079</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H45" s="4">
+        <v>10</v>
+      </c>
+      <c r="I45" s="4" t="s">
+        <v>1150</v>
+      </c>
+      <c r="J45" s="4">
+        <v>2</v>
+      </c>
+      <c r="K45" s="4" t="s">
+        <v>1196</v>
+      </c>
+      <c r="L45" s="4">
+        <v>1</v>
+      </c>
+      <c r="M45" s="4">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="N31" s="4" t="s">
+      <c r="N45" s="4" t="s">
+        <v>1146</v>
+      </c>
+      <c r="O45" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="O31" s="4" t="s">
+      <c r="P45" s="4" t="str">
+        <f>VLOOKUP((H45&amp;J45&amp;L45),AP_lookup_table!D31:E1030,2,FALSE)</f>
+        <v>L</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
+        <v>1161</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>1104</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>1152</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>1136</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>1164</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>1027</v>
+      </c>
+      <c r="H46" s="4">
+        <v>1</v>
+      </c>
+      <c r="I46" s="4" t="s">
+        <v>1103</v>
+      </c>
+      <c r="J46" s="4">
+        <v>1</v>
+      </c>
+      <c r="K46" s="4" t="s">
+        <v>1147</v>
+      </c>
+      <c r="L46" s="4">
+        <v>3</v>
+      </c>
+      <c r="M46" s="4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="N46" s="4" t="s">
+        <v>1146</v>
+      </c>
+      <c r="O46" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="P31" s="4" t="str">
-        <f>VLOOKUP((H31&amp;J31&amp;L31),AP_lookup_table!D16:E1015,2,FALSE)</f>
+      <c r="P46" s="4" t="str">
+        <f>VLOOKUP((H46&amp;J46&amp;L46),AP_lookup_table!D32:E1031,2,FALSE)</f>
         <v>L</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
-        <v>1109</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>1104</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>1111</v>
-      </c>
-      <c r="D32" s="4" t="s">
+    <row r="47" spans="1:16" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="4" t="s">
+        <v>1162</v>
+      </c>
+      <c r="B47" s="4" t="s">
         <v>1106</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="C47" s="4" t="s">
+        <v>1144</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>1155</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>1156</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>1157</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>1027</v>
+      </c>
+      <c r="H47" s="4">
+        <v>1</v>
+      </c>
+      <c r="I47" s="4" t="s">
+        <v>1158</v>
+      </c>
+      <c r="J47" s="4">
+        <v>1</v>
+      </c>
+      <c r="K47" s="4" t="s">
+        <v>1062</v>
+      </c>
+      <c r="L47" s="4">
+        <v>1</v>
+      </c>
+      <c r="M47" s="4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N47" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="O47" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="P47" s="4" t="str">
+        <f>VLOOKUP((H47&amp;J47&amp;L47),AP_lookup_table!D33:E1032,2,FALSE)</f>
+        <v>L</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="s">
+        <v>1163</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>1144</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>1153</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>1148</v>
+      </c>
+      <c r="F48" s="4" t="s">
         <v>1149</v>
       </c>
-      <c r="F32" s="4" t="s">
-        <v>1146</v>
-      </c>
-      <c r="G32" s="4" t="s">
+      <c r="G48" s="4" t="s">
         <v>1027</v>
       </c>
-      <c r="H32" s="4">
-        <v>1</v>
-      </c>
-      <c r="I32" s="4" t="s">
-        <v>1108</v>
-      </c>
-      <c r="J32" s="4">
-        <v>1</v>
-      </c>
-      <c r="K32" s="4" t="s">
+      <c r="H48" s="4">
+        <v>1</v>
+      </c>
+      <c r="I48" s="4" t="s">
+        <v>1159</v>
+      </c>
+      <c r="J48" s="4">
+        <v>2</v>
+      </c>
+      <c r="K48" s="4" t="s">
         <v>1062</v>
       </c>
-      <c r="L32" s="4">
-        <v>3</v>
-      </c>
-      <c r="M32" s="4">
+      <c r="L48" s="4">
+        <v>1</v>
+      </c>
+      <c r="M48" s="4">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="N32" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="N48" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="O32" s="4" t="s">
+      <c r="O48" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="P32" s="4" t="str">
-        <f>VLOOKUP((H32&amp;J32&amp;L32),AP_lookup_table!D17:E1016,2,FALSE)</f>
+      <c r="P48" s="4" t="str">
+        <f>VLOOKUP((H48&amp;J48&amp;L48),AP_lookup_table!D34:E1033,2,FALSE)</f>
         <v>L</v>
       </c>
-    </row>
-    <row r="33" spans="1:16" ht="116.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="4" t="s">
-        <v>1110</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>1104</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>1111</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>1107</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>1147</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>1151</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H33" s="4">
-        <v>10</v>
-      </c>
-      <c r="I33" s="4" t="s">
-        <v>1150</v>
-      </c>
-      <c r="J33" s="4">
-        <v>2</v>
-      </c>
-      <c r="K33" s="4" t="s">
-        <v>1148</v>
-      </c>
-      <c r="L33" s="4">
-        <v>1</v>
-      </c>
-      <c r="M33" s="4">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="N33" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="O33" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="P33" s="4" t="str">
-        <f>VLOOKUP((H33&amp;J33&amp;L33),AP_lookup_table!D18:E1017,2,FALSE)</f>
-        <v>L</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
-      <c r="I34" s="3"/>
-      <c r="J34" s="3"/>
-      <c r="K34" s="3"/>
-      <c r="L34" s="3"/>
-      <c r="M34" s="3"/>
-      <c r="N34" s="3"/>
-      <c r="O34" s="3"/>
-      <c r="P34" s="3"/>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
-      <c r="K35" s="3"/>
-      <c r="L35" s="3"/>
-      <c r="M35" s="3"/>
-      <c r="N35" s="3"/>
-      <c r="O35" s="3"/>
-      <c r="P35" s="3"/>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
-      <c r="I36" s="3"/>
-      <c r="J36" s="3"/>
-      <c r="K36" s="3"/>
-      <c r="L36" s="3"/>
-      <c r="M36" s="3"/>
-      <c r="N36" s="3"/>
-      <c r="O36" s="3"/>
-      <c r="P36" s="3"/>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
-      <c r="K37" s="3"/>
-      <c r="L37" s="3"/>
-      <c r="M37" s="3"/>
-      <c r="N37" s="3"/>
-      <c r="O37" s="3"/>
-      <c r="P37" s="3"/>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="3"/>
-      <c r="J38" s="3"/>
-      <c r="K38" s="3"/>
-      <c r="L38" s="3"/>
-      <c r="M38" s="3"/>
-      <c r="N38" s="3"/>
-      <c r="O38" s="3"/>
-      <c r="P38" s="3"/>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="3"/>
-      <c r="J39" s="3"/>
-      <c r="K39" s="3"/>
-      <c r="L39" s="3"/>
-      <c r="M39" s="3"/>
-      <c r="N39" s="3"/>
-      <c r="O39" s="3"/>
-      <c r="P39" s="3"/>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
-      <c r="I40" s="3"/>
-      <c r="J40" s="3"/>
-      <c r="K40" s="3"/>
-      <c r="L40" s="3"/>
-      <c r="M40" s="3"/>
-      <c r="N40" s="3"/>
-      <c r="O40" s="3"/>
-      <c r="P40" s="3"/>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
-      <c r="I41" s="3"/>
-      <c r="J41" s="3"/>
-      <c r="K41" s="3"/>
-      <c r="L41" s="3"/>
-      <c r="M41" s="3"/>
-      <c r="N41" s="3"/>
-      <c r="O41" s="3"/>
-      <c r="P41" s="3"/>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A42" s="3"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
-      <c r="I42" s="3"/>
-      <c r="J42" s="3"/>
-      <c r="K42" s="3"/>
-      <c r="L42" s="3"/>
-      <c r="M42" s="3"/>
-      <c r="N42" s="3"/>
-      <c r="O42" s="3"/>
-      <c r="P42" s="3"/>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A43" s="3"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
-      <c r="I43" s="3"/>
-      <c r="J43" s="3"/>
-      <c r="K43" s="3"/>
-      <c r="L43" s="3"/>
-      <c r="M43" s="3"/>
-      <c r="N43" s="3"/>
-      <c r="O43" s="3"/>
-      <c r="P43" s="3"/>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A44" s="3"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
-      <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
-      <c r="I44" s="3"/>
-      <c r="J44" s="3"/>
-      <c r="K44" s="3"/>
-      <c r="L44" s="3"/>
-      <c r="M44" s="3"/>
-      <c r="N44" s="3"/>
-      <c r="O44" s="3"/>
-      <c r="P44" s="3"/>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A45" s="3"/>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
-      <c r="G45" s="3"/>
-      <c r="H45" s="3"/>
-      <c r="I45" s="3"/>
-      <c r="J45" s="3"/>
-      <c r="K45" s="3"/>
-      <c r="L45" s="3"/>
-      <c r="M45" s="3"/>
-      <c r="N45" s="3"/>
-      <c r="O45" s="3"/>
-      <c r="P45" s="3"/>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A46" s="3"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
-      <c r="G46" s="3"/>
-      <c r="H46" s="3"/>
-      <c r="I46" s="3"/>
-      <c r="J46" s="3"/>
-      <c r="K46" s="3"/>
-      <c r="L46" s="3"/>
-      <c r="M46" s="3"/>
-      <c r="N46" s="3"/>
-      <c r="O46" s="3"/>
-      <c r="P46" s="3"/>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A47" s="3"/>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
-      <c r="G47" s="3"/>
-      <c r="H47" s="3"/>
-      <c r="I47" s="3"/>
-      <c r="J47" s="3"/>
-      <c r="K47" s="3"/>
-      <c r="L47" s="3"/>
-      <c r="M47" s="3"/>
-      <c r="N47" s="3"/>
-      <c r="O47" s="3"/>
-      <c r="P47" s="3"/>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A48" s="3"/>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
-      <c r="G48" s="3"/>
-      <c r="H48" s="3"/>
-      <c r="I48" s="3"/>
-      <c r="J48" s="3"/>
-      <c r="K48" s="3"/>
-      <c r="L48" s="3"/>
-      <c r="M48" s="3"/>
-      <c r="N48" s="3"/>
-      <c r="O48" s="3"/>
-      <c r="P48" s="3"/>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
@@ -6274,16 +6951,213 @@
       <c r="O72" s="3"/>
       <c r="P72" s="3"/>
     </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A73" s="3"/>
+      <c r="B73" s="3"/>
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
+      <c r="E73" s="3"/>
+      <c r="F73" s="3"/>
+      <c r="G73" s="3"/>
+      <c r="H73" s="3"/>
+      <c r="I73" s="3"/>
+      <c r="J73" s="3"/>
+      <c r="K73" s="3"/>
+      <c r="L73" s="3"/>
+      <c r="M73" s="3"/>
+      <c r="N73" s="3"/>
+      <c r="O73" s="3"/>
+      <c r="P73" s="3"/>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A74" s="3"/>
+      <c r="B74" s="3"/>
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
+      <c r="E74" s="3"/>
+      <c r="F74" s="3"/>
+      <c r="G74" s="3"/>
+      <c r="H74" s="3"/>
+      <c r="I74" s="3"/>
+      <c r="J74" s="3"/>
+      <c r="K74" s="3"/>
+      <c r="L74" s="3"/>
+      <c r="M74" s="3"/>
+      <c r="N74" s="3"/>
+      <c r="O74" s="3"/>
+      <c r="P74" s="3"/>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A75" s="3"/>
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
+      <c r="F75" s="3"/>
+      <c r="G75" s="3"/>
+      <c r="H75" s="3"/>
+      <c r="I75" s="3"/>
+      <c r="J75" s="3"/>
+      <c r="K75" s="3"/>
+      <c r="L75" s="3"/>
+      <c r="M75" s="3"/>
+      <c r="N75" s="3"/>
+      <c r="O75" s="3"/>
+      <c r="P75" s="3"/>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A76" s="3"/>
+      <c r="B76" s="3"/>
+      <c r="C76" s="3"/>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
+      <c r="F76" s="3"/>
+      <c r="G76" s="3"/>
+      <c r="H76" s="3"/>
+      <c r="I76" s="3"/>
+      <c r="J76" s="3"/>
+      <c r="K76" s="3"/>
+      <c r="L76" s="3"/>
+      <c r="M76" s="3"/>
+      <c r="N76" s="3"/>
+      <c r="O76" s="3"/>
+      <c r="P76" s="3"/>
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A77" s="3"/>
+      <c r="B77" s="3"/>
+      <c r="C77" s="3"/>
+      <c r="D77" s="3"/>
+      <c r="E77" s="3"/>
+      <c r="F77" s="3"/>
+      <c r="G77" s="3"/>
+      <c r="H77" s="3"/>
+      <c r="I77" s="3"/>
+      <c r="J77" s="3"/>
+      <c r="K77" s="3"/>
+      <c r="L77" s="3"/>
+      <c r="M77" s="3"/>
+      <c r="N77" s="3"/>
+      <c r="O77" s="3"/>
+      <c r="P77" s="3"/>
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A78" s="3"/>
+      <c r="B78" s="3"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="3"/>
+      <c r="E78" s="3"/>
+      <c r="F78" s="3"/>
+      <c r="G78" s="3"/>
+      <c r="H78" s="3"/>
+      <c r="I78" s="3"/>
+      <c r="J78" s="3"/>
+      <c r="K78" s="3"/>
+      <c r="L78" s="3"/>
+      <c r="M78" s="3"/>
+      <c r="N78" s="3"/>
+      <c r="O78" s="3"/>
+      <c r="P78" s="3"/>
+    </row>
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A79" s="3"/>
+      <c r="B79" s="3"/>
+      <c r="C79" s="3"/>
+      <c r="D79" s="3"/>
+      <c r="E79" s="3"/>
+      <c r="F79" s="3"/>
+      <c r="G79" s="3"/>
+      <c r="H79" s="3"/>
+      <c r="I79" s="3"/>
+      <c r="J79" s="3"/>
+      <c r="K79" s="3"/>
+      <c r="L79" s="3"/>
+      <c r="M79" s="3"/>
+      <c r="N79" s="3"/>
+      <c r="O79" s="3"/>
+      <c r="P79" s="3"/>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A80" s="3"/>
+      <c r="B80" s="3"/>
+      <c r="C80" s="3"/>
+      <c r="D80" s="3"/>
+      <c r="E80" s="3"/>
+      <c r="F80" s="3"/>
+      <c r="G80" s="3"/>
+      <c r="H80" s="3"/>
+      <c r="I80" s="3"/>
+      <c r="J80" s="3"/>
+      <c r="K80" s="3"/>
+      <c r="L80" s="3"/>
+      <c r="M80" s="3"/>
+      <c r="N80" s="3"/>
+      <c r="O80" s="3"/>
+      <c r="P80" s="3"/>
+    </row>
+    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A81" s="3"/>
+      <c r="B81" s="3"/>
+      <c r="C81" s="3"/>
+      <c r="D81" s="3"/>
+      <c r="E81" s="3"/>
+      <c r="F81" s="3"/>
+      <c r="G81" s="3"/>
+      <c r="H81" s="3"/>
+      <c r="I81" s="3"/>
+      <c r="J81" s="3"/>
+      <c r="K81" s="3"/>
+      <c r="L81" s="3"/>
+      <c r="M81" s="3"/>
+      <c r="N81" s="3"/>
+      <c r="O81" s="3"/>
+      <c r="P81" s="3"/>
+    </row>
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A82" s="3"/>
+      <c r="B82" s="3"/>
+      <c r="C82" s="3"/>
+      <c r="D82" s="3"/>
+      <c r="E82" s="3"/>
+      <c r="F82" s="3"/>
+      <c r="G82" s="3"/>
+      <c r="H82" s="3"/>
+      <c r="I82" s="3"/>
+      <c r="J82" s="3"/>
+      <c r="K82" s="3"/>
+      <c r="L82" s="3"/>
+      <c r="M82" s="3"/>
+      <c r="N82" s="3"/>
+      <c r="O82" s="3"/>
+      <c r="P82" s="3"/>
+    </row>
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A83" s="3"/>
+      <c r="B83" s="3"/>
+      <c r="C83" s="3"/>
+      <c r="D83" s="3"/>
+      <c r="E83" s="3"/>
+      <c r="F83" s="3"/>
+      <c r="G83" s="3"/>
+      <c r="H83" s="3"/>
+      <c r="I83" s="3"/>
+      <c r="J83" s="3"/>
+      <c r="K83" s="3"/>
+      <c r="L83" s="3"/>
+      <c r="M83" s="3"/>
+      <c r="N83" s="3"/>
+      <c r="O83" s="3"/>
+      <c r="P83" s="3"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
     <mergeCell ref="A1:O1"/>
-    <mergeCell ref="A17:P17"/>
+    <mergeCell ref="A31:P31"/>
     <mergeCell ref="A3:P3"/>
-    <mergeCell ref="A30:P30"/>
-    <mergeCell ref="A15:P15"/>
+    <mergeCell ref="A20:P20"/>
   </mergeCells>
-  <conditionalFormatting sqref="H4:H16 J4:J16 L4:L16 L18:L29 J18:J29 H18:H29 L31:L125 H31:H125 J31:J125">
-    <cfRule type="colorScale" priority="10">
+  <conditionalFormatting sqref="H45:H136 J45:J136 L45:L136 H4:H25 J4:J25 L4:L25 H27:H30 J27:J30 L27:L30">
+    <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="num" val="1"/>
         <cfvo type="num" val="5"/>
@@ -6294,8 +7168,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L16 J16 H16">
-    <cfRule type="colorScale" priority="5">
+  <conditionalFormatting sqref="L32:L44 J32:J44 H32:H44">
+    <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="num" val="1"/>
         <cfvo type="num" val="5"/>
@@ -6306,8 +7180,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M4:M16 M18:M29 M31:M33 A30">
-    <cfRule type="colorScale" priority="6">
+  <conditionalFormatting sqref="M4:M26">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="num" val="1"/>
         <cfvo type="num" val="500"/>
@@ -6318,8 +7192,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M16">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="M32:M44">
+    <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="num" val="1"/>
         <cfvo type="num" val="500"/>
@@ -6330,26 +7204,62 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P4:P16">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+  <conditionalFormatting sqref="P45:P136 P4:P30">
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="9" operator="equal">
       <formula>"M"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="10" operator="equal">
       <formula>"L"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P18:P29 P31:P125">
-    <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
+  <conditionalFormatting sqref="P32:P44">
+    <cfRule type="cellIs" dxfId="2" priority="13" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="14" operator="equal">
       <formula>"M"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="15" operator="equal">
       <formula>"L"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M45:M48">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="500"/>
+        <cfvo type="num" val="1000"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L26 J26 H26">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="5"/>
+        <cfvo type="num" val="10"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M27:M30">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="500"/>
+        <cfvo type="num" val="1000"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
DFMEA: Add pdf export
</commit_message>
<xml_diff>
--- a/docs/anchor_DFMEA.xlsx
+++ b/docs/anchor_DFMEA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmatt\Documents\anchor\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{227354BB-CF86-4EA9-BBEA-9B40EE7A00CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A23B92F-AD28-43D4-82F5-63EAD2327EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{6E08087A-9028-4EA2-B63F-382C2D4CF040}"/>
   </bookViews>
@@ -3770,28 +3770,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF63BE7B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB84"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8696B"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -4130,10 +4109,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20939D60-F13B-4603-AAC1-1CA252B6FC6A}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:P83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7158,6 +7140,18 @@
   </mergeCells>
   <conditionalFormatting sqref="H45:H136 J45:J136 L45:L136 H4:H25 J4:J25 L4:L25 H27:H30 J27:J30 L27:L30">
     <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="5"/>
+        <cfvo type="num" val="10"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L26 J26 H26">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="1"/>
         <cfvo type="num" val="5"/>
@@ -7192,6 +7186,18 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="M27:M30">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="500"/>
+        <cfvo type="num" val="1000"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="M32:M44">
     <cfRule type="colorScale" priority="12">
       <colorScale>
@@ -7202,28 +7208,6 @@
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
       </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P45:P136 P4:P30">
-    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
-      <formula>"H"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="9" operator="equal">
-      <formula>"M"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="10" operator="equal">
-      <formula>"L"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P32:P44">
-    <cfRule type="cellIs" dxfId="2" priority="13" operator="equal">
-      <formula>"H"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="14" operator="equal">
-      <formula>"M"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="15" operator="equal">
-      <formula>"L"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M45:M48">
@@ -7238,32 +7222,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L26 J26 H26">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="num" val="1"/>
-        <cfvo type="num" val="5"/>
-        <cfvo type="num" val="10"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
+  <conditionalFormatting sqref="P4:P30 P32:P136">
+    <cfRule type="cellIs" dxfId="2" priority="8" operator="equal">
+      <formula>"H"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="9" operator="equal">
+      <formula>"M"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="10" operator="equal">
+      <formula>"L"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M27:M30">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="num" val="1"/>
-        <cfvo type="num" val="500"/>
-        <cfvo type="num" val="1000"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="42" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
schematic: wire up contactors
</commit_message>
<xml_diff>
--- a/docs/anchor_DFMEA.xlsx
+++ b/docs/anchor_DFMEA.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmatt\Documents\anchor\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A23B92F-AD28-43D4-82F5-63EAD2327EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18F056D6-4D42-4E09-8DB5-2F943A3F9F17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{6E08087A-9028-4EA2-B63F-382C2D4CF040}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2496" uniqueCount="1198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2496" uniqueCount="1199">
   <si>
     <t>Ref ID</t>
   </si>
@@ -3352,9 +3352,6 @@
     <t>PTC Heater</t>
   </si>
   <si>
-    <t>Heater Bed Assy</t>
-  </si>
-  <si>
     <t>Chamber Heater Assy</t>
   </si>
   <si>
@@ -3620,6 +3617,12 @@
   </si>
   <si>
     <t>Thermal fuse on bed heater; Thermal fuse on bed SSR; Current fuse on bed SSR; Thermistor on heater + SW control loop; Klipper/moonraker timeout on RPI</t>
+  </si>
+  <si>
+    <t>Ensure heatsink can dissipate more energy than it would take for the current fuse to blow</t>
+  </si>
+  <si>
+    <t>Heated Bed Assy</t>
   </si>
 </sst>
 </file>
@@ -4115,7 +4118,7 @@
   <dimension ref="A1:P83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4211,7 +4214,7 @@
     </row>
     <row r="3" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
-        <v>1108</v>
+        <v>1198</v>
       </c>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
@@ -4344,7 +4347,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>1055</v>
@@ -4396,13 +4399,13 @@
         <v>5</v>
       </c>
       <c r="D7" s="4" t="s">
+        <v>1174</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>1175</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>1176</v>
-      </c>
       <c r="F7" s="4" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>1027</v>
@@ -4515,7 +4518,7 @@
         <v>6</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="J9" s="4">
         <v>2</v>
@@ -4531,7 +4534,7 @@
         <v>36</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="O9" s="4" t="s">
         <v>1071</v>
@@ -4543,7 +4546,7 @@
     </row>
     <row r="10" spans="1:16" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>1030</v>
@@ -4638,7 +4641,7 @@
         <v>12</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="P11" s="4" t="str">
         <f>VLOOKUP((H11&amp;J11&amp;L11),AP_lookup_table!D7:E1006,2,FALSE)</f>
@@ -4749,7 +4752,7 @@
         <v>L</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>1086</v>
       </c>
@@ -4794,7 +4797,7 @@
         <v>1085</v>
       </c>
       <c r="O14" s="4" t="s">
-        <v>12</v>
+        <v>1197</v>
       </c>
       <c r="P14" s="4" t="str">
         <f>VLOOKUP((H14&amp;J14&amp;L14),AP_lookup_table!D8:E1007,2,FALSE)</f>
@@ -4855,7 +4858,7 @@
     </row>
     <row r="16" spans="1:16" ht="109.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>1030</v>
@@ -4864,10 +4867,10 @@
         <v>1104</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>1079</v>
@@ -4879,13 +4882,13 @@
         <v>10</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="J16" s="4">
         <v>2</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="L16" s="4">
         <v>1</v>
@@ -4895,7 +4898,7 @@
         <v>20</v>
       </c>
       <c r="N16" s="4" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="O16" s="4" t="s">
         <v>12</v>
@@ -4907,7 +4910,7 @@
     </row>
     <row r="17" spans="1:16" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>1030</v>
@@ -4916,13 +4919,13 @@
         <v>1104</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>1027</v>
@@ -4937,7 +4940,7 @@
         <v>1</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="L17" s="4">
         <v>3</v>
@@ -4947,7 +4950,7 @@
         <v>3</v>
       </c>
       <c r="N17" s="4" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="O17" s="4" t="s">
         <v>12</v>
@@ -4959,22 +4962,22 @@
     </row>
     <row r="18" spans="1:16" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>1030</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="D18" s="4" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E18" s="4" t="s">
         <v>1155</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="F18" s="4" t="s">
         <v>1156</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>1157</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>1027</v>
@@ -4983,7 +4986,7 @@
         <v>1</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="J18" s="4">
         <v>1</v>
@@ -5011,22 +5014,22 @@
     </row>
     <row r="19" spans="1:16" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>1030</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="E19" s="4" t="s">
+        <v>1147</v>
+      </c>
+      <c r="F19" s="4" t="s">
         <v>1148</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>1149</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>1027</v>
@@ -5035,7 +5038,7 @@
         <v>1</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="J19" s="4">
         <v>2</v>
@@ -5063,7 +5066,7 @@
     </row>
     <row r="20" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="B20" s="12"/>
       <c r="C20" s="12"/>
@@ -5086,10 +5089,10 @@
         <v>1105</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>1028</v>
@@ -5113,7 +5116,7 @@
         <v>2</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="L21" s="4">
         <v>4</v>
@@ -5126,7 +5129,7 @@
         <v>1054</v>
       </c>
       <c r="O21" s="4" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="P21" s="4" t="str">
         <f>VLOOKUP((H21&amp;J21&amp;L21),AP_lookup_table!D17:E1016,2,FALSE)</f>
@@ -5135,16 +5138,16 @@
     </row>
     <row r="22" spans="1:16" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
+        <v>1164</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>1184</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>1120</v>
+      </c>
+      <c r="D22" s="4" t="s">
         <v>1165</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>1185</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>1121</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>1166</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>1052</v>
@@ -5187,16 +5190,16 @@
     </row>
     <row r="23" spans="1:16" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
+        <v>1166</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>1184</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>1120</v>
+      </c>
+      <c r="D23" s="4" t="s">
         <v>1167</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>1185</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>1121</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>1168</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>1067</v>
@@ -5211,7 +5214,7 @@
         <v>6</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="J23" s="4">
         <v>4</v>
@@ -5227,7 +5230,7 @@
         <v>72</v>
       </c>
       <c r="N23" s="4" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="O23" s="4" t="s">
         <v>1071</v>
@@ -5239,19 +5242,19 @@
     </row>
     <row r="24" spans="1:16" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>1073</v>
@@ -5289,22 +5292,22 @@
     </row>
     <row r="25" spans="1:16" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>1055</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="G25" s="4"/>
       <c r="H25" s="4">
@@ -5339,10 +5342,10 @@
     </row>
     <row r="26" spans="1:16" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>1041</v>
@@ -5379,10 +5382,10 @@
         <v>42</v>
       </c>
       <c r="N26" s="4" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="O26" s="4" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="P26" s="4" t="str">
         <f>VLOOKUP((H26&amp;J26&amp;L26),AP_lookup_table!D22:E1021,2,FALSE)</f>
@@ -5391,19 +5394,19 @@
     </row>
     <row r="27" spans="1:16" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>1104</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>1079</v>
@@ -5415,13 +5418,13 @@
         <v>10</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="J27" s="4">
         <v>2</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="L27" s="4">
         <v>4</v>
@@ -5431,7 +5434,7 @@
         <v>80</v>
       </c>
       <c r="N27" s="4" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="O27" s="4" t="s">
         <v>12</v>
@@ -5443,22 +5446,22 @@
     </row>
     <row r="28" spans="1:16" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>1104</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>1027</v>
@@ -5473,7 +5476,7 @@
         <v>1</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="L28" s="4">
         <v>3</v>
@@ -5483,7 +5486,7 @@
         <v>3</v>
       </c>
       <c r="N28" s="4" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="O28" s="4" t="s">
         <v>12</v>
@@ -5495,22 +5498,22 @@
     </row>
     <row r="29" spans="1:16" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="D29" s="4" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E29" s="4" t="s">
         <v>1155</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="F29" s="4" t="s">
         <v>1156</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>1157</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>1027</v>
@@ -5519,7 +5522,7 @@
         <v>1</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="J29" s="4">
         <v>1</v>
@@ -5547,22 +5550,22 @@
     </row>
     <row r="30" spans="1:16" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="E30" s="4" t="s">
+        <v>1147</v>
+      </c>
+      <c r="F30" s="4" t="s">
         <v>1148</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>1149</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>1027</v>
@@ -5571,7 +5574,7 @@
         <v>1</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="J30" s="4">
         <v>2</v>
@@ -5599,7 +5602,7 @@
     </row>
     <row r="31" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12"/>
@@ -5619,7 +5622,7 @@
     </row>
     <row r="32" spans="1:16" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>1106</v>
@@ -5671,7 +5674,7 @@
     </row>
     <row r="33" spans="1:16" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>1106</v>
@@ -5695,7 +5698,7 @@
         <v>2</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="J33" s="4">
         <v>2</v>
@@ -5723,7 +5726,7 @@
     </row>
     <row r="34" spans="1:16" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>1106</v>
@@ -5732,13 +5735,13 @@
         <v>1107</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>1055</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>1027</v>
@@ -5747,7 +5750,7 @@
         <v>1</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="J34" s="4">
         <v>4</v>
@@ -5775,7 +5778,7 @@
     </row>
     <row r="35" spans="1:16" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>1106</v>
@@ -5784,10 +5787,10 @@
         <v>1107</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="F35" s="4" t="s">
         <v>1073</v>
@@ -5799,7 +5802,7 @@
         <v>3</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="J35" s="4">
         <v>1</v>
@@ -5827,7 +5830,7 @@
     </row>
     <row r="36" spans="1:16" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>1106</v>
@@ -5851,7 +5854,7 @@
         <v>7</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
       <c r="J36" s="4">
         <v>3</v>
@@ -5879,7 +5882,7 @@
     </row>
     <row r="37" spans="1:16" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>1106</v>
@@ -5931,7 +5934,7 @@
     </row>
     <row r="38" spans="1:16" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>1106</v>
@@ -5940,10 +5943,10 @@
         <v>1107</v>
       </c>
       <c r="D38" s="4" t="s">
+        <v>1133</v>
+      </c>
+      <c r="E38" s="4" t="s">
         <v>1134</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>1135</v>
       </c>
       <c r="F38" s="4" t="s">
         <v>1027</v>
@@ -5955,7 +5958,7 @@
         <v>4</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="J38" s="4">
         <v>2</v>
@@ -5974,7 +5977,7 @@
         <v>12</v>
       </c>
       <c r="O38" s="4" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="P38" s="4" t="str">
         <f>VLOOKUP((H38&amp;J38&amp;L38),AP_lookup_table!D17:E1016,2,FALSE)</f>
@@ -5983,13 +5986,13 @@
     </row>
     <row r="39" spans="1:16" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>1106</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>1038</v>
@@ -6007,7 +6010,7 @@
         <v>7</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="J39" s="4">
         <v>2</v>
@@ -6026,7 +6029,7 @@
         <v>12</v>
       </c>
       <c r="O39" s="4" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="P39" s="4" t="str">
         <f>VLOOKUP((H39&amp;J39&amp;L39),AP_lookup_table!D18:E1017,2,FALSE)</f>
@@ -6035,7 +6038,7 @@
     </row>
     <row r="40" spans="1:16" ht="66.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>1106</v>
@@ -6087,7 +6090,7 @@
     </row>
     <row r="41" spans="1:16" ht="66.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>1106</v>
@@ -6137,9 +6140,9 @@
         <v>L</v>
       </c>
     </row>
-    <row r="42" spans="1:16" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16" ht="65.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>1106</v>
@@ -6182,7 +6185,7 @@
         <v>1085</v>
       </c>
       <c r="O42" s="4" t="s">
-        <v>12</v>
+        <v>1197</v>
       </c>
       <c r="P42" s="4" t="str">
         <f>VLOOKUP((H42&amp;J42&amp;L42),AP_lookup_table!D19:E1018,2,FALSE)</f>
@@ -6191,7 +6194,7 @@
     </row>
     <row r="43" spans="1:16" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>1106</v>
@@ -6243,37 +6246,37 @@
     </row>
     <row r="44" spans="1:16" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>1106</v>
       </c>
       <c r="C44" s="4" t="s">
+        <v>1122</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>1124</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>1127</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>1128</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>1129</v>
+      </c>
+      <c r="H44" s="4">
+        <v>5</v>
+      </c>
+      <c r="I44" s="4" t="s">
+        <v>1125</v>
+      </c>
+      <c r="J44" s="4">
+        <v>3</v>
+      </c>
+      <c r="K44" s="4" t="s">
         <v>1123</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>1125</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>1128</v>
-      </c>
-      <c r="F44" s="4" t="s">
-        <v>1129</v>
-      </c>
-      <c r="G44" s="4" t="s">
-        <v>1130</v>
-      </c>
-      <c r="H44" s="4">
-        <v>5</v>
-      </c>
-      <c r="I44" s="4" t="s">
-        <v>1126</v>
-      </c>
-      <c r="J44" s="4">
-        <v>3</v>
-      </c>
-      <c r="K44" s="4" t="s">
-        <v>1124</v>
       </c>
       <c r="L44" s="4">
         <v>2</v>
@@ -6283,7 +6286,7 @@
         <v>30</v>
       </c>
       <c r="N44" s="4" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="O44" s="4" t="s">
         <v>12</v>
@@ -6295,7 +6298,7 @@
     </row>
     <row r="45" spans="1:16" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>1106</v>
@@ -6304,10 +6307,10 @@
         <v>1104</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="F45" s="4" t="s">
         <v>1079</v>
@@ -6319,13 +6322,13 @@
         <v>10</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="J45" s="4">
         <v>2</v>
       </c>
       <c r="K45" s="4" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="L45" s="4">
         <v>1</v>
@@ -6335,7 +6338,7 @@
         <v>20</v>
       </c>
       <c r="N45" s="4" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="O45" s="4" t="s">
         <v>12</v>
@@ -6347,7 +6350,7 @@
     </row>
     <row r="46" spans="1:16" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>1106</v>
@@ -6356,13 +6359,13 @@
         <v>1104</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="G46" s="4" t="s">
         <v>1027</v>
@@ -6377,7 +6380,7 @@
         <v>1</v>
       </c>
       <c r="K46" s="4" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="L46" s="4">
         <v>3</v>
@@ -6387,7 +6390,7 @@
         <v>3</v>
       </c>
       <c r="N46" s="4" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="O46" s="4" t="s">
         <v>12</v>
@@ -6399,22 +6402,22 @@
     </row>
     <row r="47" spans="1:16" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>1106</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="D47" s="4" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E47" s="4" t="s">
         <v>1155</v>
       </c>
-      <c r="E47" s="4" t="s">
+      <c r="F47" s="4" t="s">
         <v>1156</v>
-      </c>
-      <c r="F47" s="4" t="s">
-        <v>1157</v>
       </c>
       <c r="G47" s="4" t="s">
         <v>1027</v>
@@ -6423,7 +6426,7 @@
         <v>1</v>
       </c>
       <c r="I47" s="4" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="J47" s="4">
         <v>1</v>
@@ -6451,22 +6454,22 @@
     </row>
     <row r="48" spans="1:16" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>1106</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="E48" s="4" t="s">
+        <v>1147</v>
+      </c>
+      <c r="F48" s="4" t="s">
         <v>1148</v>
-      </c>
-      <c r="F48" s="4" t="s">
-        <v>1149</v>
       </c>
       <c r="G48" s="4" t="s">
         <v>1027</v>
@@ -6475,7 +6478,7 @@
         <v>1</v>
       </c>
       <c r="I48" s="4" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="J48" s="4">
         <v>2</v>

</xml_diff>